<commit_message>
new gitignore rules strange and styles
</commit_message>
<xml_diff>
--- a/docs/db/Base.xlsx
+++ b/docs/db/Base.xlsx
@@ -539,19 +539,19 @@
     <t>КПУ-2Н, ниппельный, нормально открытый</t>
   </si>
   <si>
-    <t>59d08e254fd856a3999347fc9decaebd</t>
+    <t>1753277370d4ac6947b80252811a8927</t>
   </si>
   <si>
     <t>КПУ-2Н, ниппельный, нормально закрытый</t>
   </si>
   <si>
-    <t>5026141d680ec7389cc9ff1a436253a0</t>
+    <t>5b97739120375bd47c3ae50d3950e58d</t>
   </si>
   <si>
     <t>КПУ-2Н-ВД, канальный, нормально открытый</t>
   </si>
   <si>
-    <t>0b5a927f5ca0871e8381865e10b43177</t>
+    <t>dbf81601cf5c17223bea2860580b3418</t>
   </si>
   <si>
     <t>https://www.veza.ru/produktsiya/klapany-i-setevye-elementy/protivopozharnye-klapany/pryamougolnye-protivopozharnye-klapany/kpu-2n-pryamougolnye</t>
@@ -565,7 +565,7 @@
     <t>КПУ-2Н-ВД, канальный, нормально закрытый</t>
   </si>
   <si>
-    <t>95552d5b1b1c47a3531781219083398c</t>
+    <t>280c6fce5b59c62e1dfd48172a2b4057</t>
   </si>
   <si>
     <t>1xЭП: 100x100...1000x1500;
@@ -1200,10 +1200,10 @@
     <t>(150x150)x(100x100)...(2000x1400)x(1400x1400)</t>
   </si>
   <si>
-    <t>Воздуховод (Размер, Скорость, Расход, Потеря давления)</t>
-  </si>
-  <si>
-    <t>7f5d79c664692bc497ba2e990b66e08d</t>
+    <t>Воздуховод (4 параметра)</t>
+  </si>
+  <si>
+    <t>b3fecc43137e617af4aa576ec4217dee</t>
   </si>
   <si>
     <t>Выноска автоматически определяет форму воздуховода и делает выбор между обозначением круглого и прямоугольного воздуховодов</t>
@@ -3840,8 +3840,8 @@
   <sheetPr/>
   <dimension ref="B4:V113"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="J92" workbookViewId="0">
-      <selection activeCell="P109" sqref="P109"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -8468,11 +8468,8 @@
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F108;F5:F86;F97:F107;F109:F113">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F86;F97:F113">
       <formula1>Категория_сайта</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K108;K5:K83;K96:K107;K109:K113">
-      <formula1>Тип_графики</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G78">
       <formula1>Категория_техническая</formula1>
@@ -8482,6 +8479,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J52;J109:J113">
       <formula1>Производитель</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5:K83;K96:K113">
+      <formula1>Тип_графики</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q5:V93;Q97:V113">
       <formula1>"ДА"</formula1>
@@ -9444,7 +9444,7 @@
       </c>
       <c r="E15" t="str">
         <f>IF(Компоненты!E15&lt;&gt;"",Компоненты!E15,"")</f>
-        <v>59d08e254fd856a3999347fc9decaebd</v>
+        <v>1753277370d4ac6947b80252811a8927</v>
       </c>
       <c r="F15" t="str">
         <f>IF(Компоненты!F15&lt;&gt;"",Компоненты!F15,"")</f>
@@ -9528,7 +9528,7 @@
       </c>
       <c r="E16" t="str">
         <f>IF(Компоненты!E16&lt;&gt;"",Компоненты!E16,"")</f>
-        <v>5026141d680ec7389cc9ff1a436253a0</v>
+        <v>5b97739120375bd47c3ae50d3950e58d</v>
       </c>
       <c r="F16" t="str">
         <f>IF(Компоненты!F16&lt;&gt;"",Компоненты!F16,"")</f>
@@ -9612,7 +9612,7 @@
       </c>
       <c r="E17" t="str">
         <f>IF(Компоненты!E17&lt;&gt;"",Компоненты!E17,"")</f>
-        <v>0b5a927f5ca0871e8381865e10b43177</v>
+        <v>dbf81601cf5c17223bea2860580b3418</v>
       </c>
       <c r="F17" t="str">
         <f>IF(Компоненты!F17&lt;&gt;"",Компоненты!F17,"")</f>
@@ -9696,7 +9696,7 @@
       </c>
       <c r="E18" t="str">
         <f>IF(Компоненты!E18&lt;&gt;"",Компоненты!E18,"")</f>
-        <v>95552d5b1b1c47a3531781219083398c</v>
+        <v>280c6fce5b59c62e1dfd48172a2b4057</v>
       </c>
       <c r="F18" t="str">
         <f>IF(Компоненты!F18&lt;&gt;"",Компоненты!F18,"")</f>
@@ -15115,7 +15115,7 @@
       </c>
       <c r="C84" t="str">
         <f>IF(Компоненты!C84&lt;&gt;"",Компоненты!C84,"")</f>
-        <v>Воздуховод (Размер, Скорость, Расход, Потеря давления)</v>
+        <v>Воздуховод (4 параметра)</v>
       </c>
       <c r="D84">
         <f>IF(Компоненты!D84&lt;&gt;"",Компоненты!D84,"")</f>
@@ -15123,7 +15123,7 @@
       </c>
       <c r="E84" t="str">
         <f>IF(Компоненты!E84&lt;&gt;"",Компоненты!E84,"")</f>
-        <v>7f5d79c664692bc497ba2e990b66e08d</v>
+        <v>b3fecc43137e617af4aa576ec4217dee</v>
       </c>
       <c r="F84" t="str">
         <f>IF(Компоненты!F84&lt;&gt;"",Компоненты!F84,"")</f>

</xml_diff>

<commit_message>
chiller and drycooler added
</commit_message>
<xml_diff>
--- a/docs/db/Base.xlsx
+++ b/docs/db/Base.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9000" activeTab="3"/>
+    <workbookView windowWidth="29868" windowHeight="13320" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Параметры_компонентов" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1468" uniqueCount="470">
   <si>
     <t>На этом листе собраны возможные значения параметров, описывающих типы компонентов nanoCAD BIM Вентиляция</t>
   </si>
@@ -442,7 +442,7 @@
     <t>АМН</t>
   </si>
   <si>
-    <t>f6aa636a735baf77feb3c1f1df96980f</t>
+    <t>e5a6688b3270328e37bc280a5ea313f8</t>
   </si>
   <si>
     <t>жалюзийная</t>
@@ -1482,6 +1482,42 @@
   </si>
   <si>
     <t>2024.08.30</t>
+  </si>
+  <si>
+    <t>Чиллер модульный</t>
+  </si>
+  <si>
+    <t>e805835f79ab0c20004fee239013904b</t>
+  </si>
+  <si>
+    <t>Чиллер</t>
+  </si>
+  <si>
+    <t>воздушный</t>
+  </si>
+  <si>
+    <t>Параметризованы все основные габариты и патрубки воды</t>
+  </si>
+  <si>
+    <t>45...188 кВт</t>
+  </si>
+  <si>
+    <t>2024.10.21</t>
+  </si>
+  <si>
+    <t>Драйкулер V-образный</t>
+  </si>
+  <si>
+    <t>0dcbe09a0bf3debac6e01b14026d511a</t>
+  </si>
+  <si>
+    <t>Драйкулер</t>
+  </si>
+  <si>
+    <t>V-образный</t>
+  </si>
+  <si>
+    <t>91...131 кВт</t>
   </si>
 </sst>
 </file>
@@ -3841,8 +3877,8 @@
   <sheetPr/>
   <dimension ref="B4:V113"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="E97" sqref="E97"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="G111" sqref="G111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -8433,19 +8469,93 @@
         <v>457</v>
       </c>
     </row>
-    <row r="109" ht="15" customHeight="1" spans="5:16">
-      <c r="E109" s="2"/>
-      <c r="L109" s="5"/>
-      <c r="N109" s="4"/>
-      <c r="O109" s="5"/>
-      <c r="P109" s="10"/>
-    </row>
-    <row r="110" ht="15" customHeight="1" spans="5:16">
-      <c r="E110" s="2"/>
-      <c r="L110" s="5"/>
-      <c r="N110" s="4"/>
-      <c r="O110" s="5"/>
-      <c r="P110" s="10"/>
+    <row r="109" ht="15" customHeight="1" spans="2:16">
+      <c r="B109" s="1">
+        <v>106</v>
+      </c>
+      <c r="C109" t="s">
+        <v>458</v>
+      </c>
+      <c r="D109">
+        <v>1</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="F109" t="s">
+        <v>30</v>
+      </c>
+      <c r="G109" t="s">
+        <v>460</v>
+      </c>
+      <c r="H109" t="s">
+        <v>461</v>
+      </c>
+      <c r="I109" t="s">
+        <v>15</v>
+      </c>
+      <c r="J109" t="s">
+        <v>29</v>
+      </c>
+      <c r="K109" t="s">
+        <v>21</v>
+      </c>
+      <c r="L109" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="N109" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="O109" s="5" t="s">
+        <v>463</v>
+      </c>
+      <c r="P109" s="6" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="110" ht="15" customHeight="1" spans="2:16">
+      <c r="B110" s="1">
+        <v>107</v>
+      </c>
+      <c r="C110" t="s">
+        <v>465</v>
+      </c>
+      <c r="D110">
+        <v>1</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="F110" t="s">
+        <v>30</v>
+      </c>
+      <c r="G110" t="s">
+        <v>467</v>
+      </c>
+      <c r="H110" t="s">
+        <v>468</v>
+      </c>
+      <c r="I110" t="s">
+        <v>15</v>
+      </c>
+      <c r="J110" t="s">
+        <v>29</v>
+      </c>
+      <c r="K110" t="s">
+        <v>21</v>
+      </c>
+      <c r="L110" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="N110" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="O110" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="P110" s="6" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="111" ht="15" customHeight="1" spans="5:16">
       <c r="E111" s="2"/>
@@ -8469,20 +8579,20 @@
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F86;F97:F113">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J109;J110;J5:J52;J111:J113">
+      <formula1>Производитель</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F110;F5:F86;F97:F109;F111:F113">
       <formula1>Категория_сайта</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I110;I5:I83;I97:I105;I107:I109;I111:I113">
+      <formula1>Форма</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K110;K5:K83;K96:K109;K111:K113">
+      <formula1>Тип_графики</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G78">
       <formula1>Категория_техническая</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I83;I97:I105;I107:I113">
-      <formula1>Форма</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J52;J109:J113">
-      <formula1>Производитель</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5:K83;K96:K113">
-      <formula1>Тип_графики</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q5:V93;Q97:V113">
       <formula1>"ДА"</formula1>
@@ -8690,7 +8800,7 @@
       </c>
       <c r="E6" t="str">
         <f>IF(Компоненты!E6&lt;&gt;"",Компоненты!E6,"")</f>
-        <v>f6aa636a735baf77feb3c1f1df96980f</v>
+        <v>e5a6688b3270328e37bc280a5ea313f8</v>
       </c>
       <c r="F6" t="str">
         <f>IF(Компоненты!F6&lt;&gt;"",Компоненты!F6,"")</f>
@@ -17166,49 +17276,49 @@
       </c>
     </row>
     <row r="109" spans="2:21">
-      <c r="B109" t="str">
+      <c r="B109">
         <f>IF(Компоненты!B109&lt;&gt;"",Компоненты!B109,"")</f>
-        <v/>
+        <v>106</v>
       </c>
       <c r="C109" t="str">
         <f>IF(Компоненты!C109&lt;&gt;"",Компоненты!C109,"")</f>
-        <v/>
-      </c>
-      <c r="D109" t="str">
+        <v>Чиллер модульный</v>
+      </c>
+      <c r="D109">
         <f>IF(Компоненты!D109&lt;&gt;"",Компоненты!D109,"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="E109" t="str">
         <f>IF(Компоненты!E109&lt;&gt;"",Компоненты!E109,"")</f>
-        <v/>
+        <v>e805835f79ab0c20004fee239013904b</v>
       </c>
       <c r="F109" t="str">
         <f>IF(Компоненты!F109&lt;&gt;"",Компоненты!F109,"")</f>
-        <v/>
+        <v>Оборудование</v>
       </c>
       <c r="G109" t="str">
         <f>IF(Компоненты!G109&lt;&gt;"",Компоненты!G109,"")</f>
-        <v/>
+        <v>Чиллер</v>
       </c>
       <c r="H109" t="str">
         <f>IF(Компоненты!H109&lt;&gt;"",Компоненты!H109,"")</f>
-        <v/>
+        <v>воздушный</v>
       </c>
       <c r="I109" t="str">
         <f>IF(Компоненты!I109&lt;&gt;"",Компоненты!I109,"")</f>
-        <v/>
+        <v>Круглый</v>
       </c>
       <c r="J109" t="str">
         <f>IF(Компоненты!J109&lt;&gt;"",Компоненты!J109,"")</f>
-        <v/>
+        <v>Базовое оборудование</v>
       </c>
       <c r="K109" t="str">
         <f>IF(Компоненты!K109&lt;&gt;"",Компоненты!K109,"")</f>
-        <v/>
+        <v>Параметрическая</v>
       </c>
       <c r="L109" t="str">
         <f>IF(Компоненты!L109&lt;&gt;"",Компоненты!L109,"")</f>
-        <v/>
+        <v>Параметризованы все основные габариты и патрубки воды</v>
       </c>
       <c r="M109" t="str">
         <f>IF(Компоненты!M109&lt;&gt;"",Компоненты!M109,"")</f>
@@ -17216,15 +17326,15 @@
       </c>
       <c r="N109" t="str">
         <f>IF(Компоненты!N109&lt;&gt;"",Компоненты!N109,"")</f>
-        <v/>
+        <v>https://www.nanocad.ru/products/bim/ventilation/</v>
       </c>
       <c r="O109" t="str">
         <f>IF(Компоненты!O109&lt;&gt;"",Компоненты!O109,"")</f>
-        <v/>
+        <v>45...188 кВт</v>
       </c>
       <c r="P109" t="str">
         <f>IF(Компоненты!P109&lt;&gt;"",Компоненты!P109,"")</f>
-        <v/>
+        <v>2024.10.21</v>
       </c>
       <c r="Q109" t="str">
         <f>IF(Компоненты!Q109&lt;&gt;"",Компоненты!Q109,"")</f>
@@ -17248,49 +17358,49 @@
       </c>
     </row>
     <row r="110" spans="2:21">
-      <c r="B110" t="str">
+      <c r="B110">
         <f>IF(Компоненты!B110&lt;&gt;"",Компоненты!B110,"")</f>
-        <v/>
+        <v>107</v>
       </c>
       <c r="C110" t="str">
         <f>IF(Компоненты!C110&lt;&gt;"",Компоненты!C110,"")</f>
-        <v/>
-      </c>
-      <c r="D110" t="str">
+        <v>Драйкулер V-образный</v>
+      </c>
+      <c r="D110">
         <f>IF(Компоненты!D110&lt;&gt;"",Компоненты!D110,"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="E110" t="str">
         <f>IF(Компоненты!E110&lt;&gt;"",Компоненты!E110,"")</f>
-        <v/>
+        <v>0dcbe09a0bf3debac6e01b14026d511a</v>
       </c>
       <c r="F110" t="str">
         <f>IF(Компоненты!F110&lt;&gt;"",Компоненты!F110,"")</f>
-        <v/>
+        <v>Оборудование</v>
       </c>
       <c r="G110" t="str">
         <f>IF(Компоненты!G110&lt;&gt;"",Компоненты!G110,"")</f>
-        <v/>
+        <v>Драйкулер</v>
       </c>
       <c r="H110" t="str">
         <f>IF(Компоненты!H110&lt;&gt;"",Компоненты!H110,"")</f>
-        <v/>
+        <v>V-образный</v>
       </c>
       <c r="I110" t="str">
         <f>IF(Компоненты!I110&lt;&gt;"",Компоненты!I110,"")</f>
-        <v/>
+        <v>Круглый</v>
       </c>
       <c r="J110" t="str">
         <f>IF(Компоненты!J110&lt;&gt;"",Компоненты!J110,"")</f>
-        <v/>
+        <v>Базовое оборудование</v>
       </c>
       <c r="K110" t="str">
         <f>IF(Компоненты!K110&lt;&gt;"",Компоненты!K110,"")</f>
-        <v/>
+        <v>Параметрическая</v>
       </c>
       <c r="L110" t="str">
         <f>IF(Компоненты!L110&lt;&gt;"",Компоненты!L110,"")</f>
-        <v/>
+        <v>Параметризованы все основные габариты и патрубки воды</v>
       </c>
       <c r="M110" t="str">
         <f>IF(Компоненты!M110&lt;&gt;"",Компоненты!M110,"")</f>
@@ -17298,15 +17408,15 @@
       </c>
       <c r="N110" t="str">
         <f>IF(Компоненты!N110&lt;&gt;"",Компоненты!N110,"")</f>
-        <v/>
+        <v>https://www.nanocad.ru/products/bim/ventilation/</v>
       </c>
       <c r="O110" t="str">
         <f>IF(Компоненты!O110&lt;&gt;"",Компоненты!O110,"")</f>
-        <v/>
+        <v>91...131 кВт</v>
       </c>
       <c r="P110" t="str">
         <f>IF(Компоненты!P110&lt;&gt;"",Компоненты!P110,"")</f>
-        <v/>
+        <v>2024.10.21</v>
       </c>
       <c r="Q110" t="str">
         <f>IF(Компоненты!Q110&lt;&gt;"",Компоненты!Q110,"")</f>

</xml_diff>

<commit_message>
db add for 111, 112
</commit_message>
<xml_diff>
--- a/docs/db/Base.xlsx
+++ b/docs/db/Base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\evoslib\public\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F749E8-71E3-4109-8A36-C59D2E238C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC12EF12-8852-4013-AB3A-AEAA092BF592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1510" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1534" uniqueCount="495">
   <si>
     <t>На этом листе собраны возможные значения параметров, описывающих типы компонентов nanoCAD BIM Вентиляция</t>
   </si>
@@ -1516,9 +1516,6 @@
     <t>Драйкулер</t>
   </si>
   <si>
-    <t>V-образный</t>
-  </si>
-  <si>
     <t>91...131 кВт</t>
   </si>
   <si>
@@ -1572,18 +1569,61 @@
   </si>
   <si>
     <t>110ab64b34191f9153caea9dd675ac38</t>
+  </si>
+  <si>
+    <t>Сплит-система</t>
+  </si>
+  <si>
+    <t>воздушного охлаждения</t>
+  </si>
+  <si>
+    <t>Параметризованы все габариты. Блок имеет патрубки для жидкостной и газовой линии, фреона и дренажа</t>
+  </si>
+  <si>
+    <t>2024.11.13</t>
+  </si>
+  <si>
+    <t>3.3…9 кВт (тепло)
+2.4…7.3 кВт (холод)</t>
+  </si>
+  <si>
+    <t>3,3…9 кВт (тепло)
+2,4…7,3 кВт (холод)</t>
+  </si>
+  <si>
+    <t>Параметризованы все габариты. Блок имеет патрубки для жидкостной и газовой линии</t>
+  </si>
+  <si>
+    <t>cf738be6c2382c779598f33b5432ad68</t>
+  </si>
+  <si>
+    <t>6e43d176a1d591209ec3727785329eb6</t>
+  </si>
+  <si>
+    <t>Сплит-система - Наружный блок</t>
+  </si>
+  <si>
+    <t>Сплит-система - Внутренний блок</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1742,11 +1782,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1756,7 +1796,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1765,13 +1805,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1">
@@ -1798,13 +1838,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1813,16 +1853,19 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2793,7 +2836,7 @@
   <dimension ref="B2:K41"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16:E24"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -3041,7 +3084,7 @@
     </row>
     <row r="24" spans="4:5">
       <c r="D24" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E24" t="s">
         <v>29</v>
@@ -3049,15 +3092,15 @@
     </row>
     <row r="25" spans="4:5">
       <c r="D25" t="s">
-        <v>37</v>
+        <v>484</v>
       </c>
       <c r="E25" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="4:5">
       <c r="D26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E26" t="s">
         <v>21</v>
@@ -3065,7 +3108,7 @@
     </row>
     <row r="27" spans="4:5">
       <c r="D27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E27" t="s">
         <v>21</v>
@@ -3073,7 +3116,7 @@
     </row>
     <row r="28" spans="4:5">
       <c r="D28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E28" t="s">
         <v>21</v>
@@ -3081,7 +3124,7 @@
     </row>
     <row r="29" spans="4:5">
       <c r="D29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E29" t="s">
         <v>21</v>
@@ -3089,7 +3132,7 @@
     </row>
     <row r="30" spans="4:5">
       <c r="D30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E30" t="s">
         <v>21</v>
@@ -3097,7 +3140,7 @@
     </row>
     <row r="31" spans="4:5">
       <c r="D31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E31" t="s">
         <v>21</v>
@@ -3105,7 +3148,7 @@
     </row>
     <row r="32" spans="4:5">
       <c r="D32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E32" t="s">
         <v>21</v>
@@ -3113,15 +3156,15 @@
     </row>
     <row r="33" spans="4:5">
       <c r="D33" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E33" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="4:5">
       <c r="D34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E34" t="s">
         <v>25</v>
@@ -3129,7 +3172,7 @@
     </row>
     <row r="35" spans="4:5">
       <c r="D35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E35" t="s">
         <v>25</v>
@@ -3137,7 +3180,7 @@
     </row>
     <row r="36" spans="4:5">
       <c r="D36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E36" t="s">
         <v>25</v>
@@ -3145,7 +3188,7 @@
     </row>
     <row r="37" spans="4:5">
       <c r="D37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E37" t="s">
         <v>25</v>
@@ -3153,9 +3196,17 @@
     </row>
     <row r="38" spans="4:5">
       <c r="D38" t="s">
+        <v>42</v>
+      </c>
+      <c r="E38" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="4:5">
+      <c r="D39" t="s">
         <v>45</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E39" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3165,7 +3216,7 @@
       </c>
       <c r="E41">
         <f>SUBTOTAL(103,Таблица_Привязка_категорий[Категория_сайта])</f>
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -3779,14 +3830,14 @@
   <dimension ref="B4:V119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E114" sqref="E114"/>
+      <pane ySplit="4" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C115" sqref="C115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="20" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" style="4" customWidth="1"/>
     <col min="6" max="6" width="19.5703125" style="1" customWidth="1"/>
@@ -9176,7 +9227,7 @@
       <c r="U109" s="11"/>
       <c r="V109" s="11"/>
     </row>
-    <row r="110" spans="2:22" ht="30">
+    <row r="110" spans="2:22" ht="60">
       <c r="B110" s="11">
         <v>107</v>
       </c>
@@ -9196,7 +9247,7 @@
         <v>466</v>
       </c>
       <c r="H110" s="11" t="s">
-        <v>467</v>
+        <v>485</v>
       </c>
       <c r="I110" s="11" t="s">
         <v>14</v>
@@ -9215,7 +9266,7 @@
         <v>302</v>
       </c>
       <c r="O110" s="11" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="P110" s="18" t="s">
         <v>463</v>
@@ -9232,13 +9283,13 @@
         <v>108</v>
       </c>
       <c r="C111" s="11" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D111" s="11">
         <v>1</v>
       </c>
       <c r="E111" s="13" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="F111" s="11" t="s">
         <v>10</v>
@@ -9247,7 +9298,7 @@
         <v>9</v>
       </c>
       <c r="H111" s="11" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="I111" s="11" t="s">
         <v>18</v>
@@ -9259,14 +9310,14 @@
         <v>20</v>
       </c>
       <c r="L111" s="11" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="M111" s="11"/>
       <c r="N111" s="17" t="s">
+        <v>472</v>
+      </c>
+      <c r="O111" s="11" t="s">
         <v>473</v>
-      </c>
-      <c r="O111" s="11" t="s">
-        <v>474</v>
       </c>
       <c r="P111" s="18" t="s">
         <v>463</v>
@@ -9283,25 +9334,25 @@
         <v>109</v>
       </c>
       <c r="C112" s="25" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D112" s="11">
         <v>1</v>
       </c>
       <c r="E112" s="13" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F112" s="11" t="s">
         <v>29</v>
       </c>
       <c r="G112" s="11" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="H112" s="25" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="I112" s="11" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J112" s="11" t="s">
         <v>28</v>
@@ -9310,17 +9361,17 @@
         <v>20</v>
       </c>
       <c r="L112" s="11" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="M112" s="11"/>
       <c r="N112" s="17" t="s">
         <v>302</v>
       </c>
       <c r="O112" s="11" t="s">
+        <v>477</v>
+      </c>
+      <c r="P112" s="24" t="s">
         <v>478</v>
-      </c>
-      <c r="P112" s="24" t="s">
-        <v>479</v>
       </c>
       <c r="Q112" s="11"/>
       <c r="R112" s="11"/>
@@ -9334,25 +9385,25 @@
         <v>110</v>
       </c>
       <c r="C113" s="25" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D113" s="11">
         <v>1</v>
       </c>
       <c r="E113" s="13" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F113" s="11" t="s">
         <v>29</v>
       </c>
       <c r="G113" s="11" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="H113" s="25" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I113" s="11" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J113" s="11" t="s">
         <v>28</v>
@@ -9361,17 +9412,17 @@
         <v>20</v>
       </c>
       <c r="L113" s="11" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="M113" s="11"/>
       <c r="N113" s="17" t="s">
         <v>302</v>
       </c>
       <c r="O113" s="25" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="P113" s="24" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="Q113" s="11"/>
       <c r="R113" s="11"/>
@@ -9380,22 +9431,48 @@
       <c r="U113" s="11"/>
       <c r="V113" s="11"/>
     </row>
-    <row r="114" spans="2:22">
-      <c r="B114" s="11"/>
-      <c r="C114" s="11"/>
-      <c r="D114" s="11"/>
-      <c r="E114" s="13"/>
-      <c r="F114" s="11"/>
-      <c r="G114" s="11"/>
+    <row r="114" spans="2:22" ht="60">
+      <c r="B114" s="11">
+        <v>111</v>
+      </c>
+      <c r="C114" s="12" t="s">
+        <v>494</v>
+      </c>
+      <c r="D114" s="11">
+        <v>1</v>
+      </c>
+      <c r="E114" s="13" t="s">
+        <v>492</v>
+      </c>
+      <c r="F114" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G114" s="11" t="s">
+        <v>484</v>
+      </c>
       <c r="H114" s="11"/>
-      <c r="I114" s="11"/>
-      <c r="J114" s="11"/>
-      <c r="K114" s="11"/>
-      <c r="L114" s="11"/>
+      <c r="I114" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="J114" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K114" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L114" s="11" t="s">
+        <v>486</v>
+      </c>
       <c r="M114" s="11"/>
-      <c r="N114" s="17"/>
-      <c r="O114" s="11"/>
-      <c r="P114" s="18"/>
+      <c r="N114" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="O114" s="11" t="s">
+        <v>488</v>
+      </c>
+      <c r="P114" s="26" t="s">
+        <v>487</v>
+      </c>
       <c r="Q114" s="11"/>
       <c r="R114" s="11"/>
       <c r="S114" s="11"/>
@@ -9403,22 +9480,48 @@
       <c r="U114" s="11"/>
       <c r="V114" s="11"/>
     </row>
-    <row r="115" spans="2:22">
-      <c r="B115" s="11"/>
-      <c r="C115" s="11"/>
-      <c r="D115" s="11"/>
-      <c r="E115" s="13"/>
-      <c r="F115" s="11"/>
-      <c r="G115" s="11"/>
+    <row r="115" spans="2:22" ht="45">
+      <c r="B115" s="11">
+        <v>112</v>
+      </c>
+      <c r="C115" s="12" t="s">
+        <v>493</v>
+      </c>
+      <c r="D115" s="11">
+        <v>1</v>
+      </c>
+      <c r="E115" s="13" t="s">
+        <v>491</v>
+      </c>
+      <c r="F115" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G115" s="11" t="s">
+        <v>484</v>
+      </c>
       <c r="H115" s="11"/>
-      <c r="I115" s="11"/>
-      <c r="J115" s="11"/>
-      <c r="K115" s="11"/>
-      <c r="L115" s="11"/>
+      <c r="I115" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="J115" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K115" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L115" s="11" t="s">
+        <v>490</v>
+      </c>
       <c r="M115" s="11"/>
-      <c r="N115" s="17"/>
-      <c r="O115" s="11"/>
-      <c r="P115" s="18"/>
+      <c r="N115" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="O115" s="11" t="s">
+        <v>489</v>
+      </c>
+      <c r="P115" s="26" t="s">
+        <v>487</v>
+      </c>
       <c r="Q115" s="11"/>
       <c r="R115" s="11"/>
       <c r="S115" s="11"/>
@@ -18321,7 +18424,7 @@
       </c>
       <c r="H110" t="str">
         <f>IF(Компоненты!H110&lt;&gt;"",Компоненты!H110,"")</f>
-        <v>V-образный</v>
+        <v>воздушного охлаждения</v>
       </c>
       <c r="I110" t="str">
         <f>IF(Компоненты!I110&lt;&gt;"",Компоненты!I110,"")</f>
@@ -18489,7 +18592,7 @@
       </c>
       <c r="I112" t="str">
         <f>IF(Компоненты!I112&lt;&gt;"",Компоненты!I112,"")</f>
-        <v>Круглый</v>
+        <v>Не применимо</v>
       </c>
       <c r="J112" t="str">
         <f>IF(Компоненты!J112&lt;&gt;"",Компоненты!J112,"")</f>
@@ -18573,7 +18676,7 @@
       </c>
       <c r="I113" t="str">
         <f>IF(Компоненты!I113&lt;&gt;"",Компоненты!I113,"")</f>
-        <v>Круглый</v>
+        <v>Не применимо</v>
       </c>
       <c r="J113" t="str">
         <f>IF(Компоненты!J113&lt;&gt;"",Компоненты!J113,"")</f>
@@ -18627,29 +18730,29 @@
       </c>
     </row>
     <row r="114" spans="2:21">
-      <c r="B114" t="str">
+      <c r="B114">
         <f>IF(Компоненты!B114&lt;&gt;"",Компоненты!B114,"")</f>
-        <v/>
+        <v>111</v>
       </c>
       <c r="C114" t="str">
         <f>IF(Компоненты!C114&lt;&gt;"",Компоненты!C114,"")</f>
-        <v/>
-      </c>
-      <c r="D114" t="str">
+        <v>Сплит-система - Внутренний блок</v>
+      </c>
+      <c r="D114">
         <f>IF(Компоненты!D114&lt;&gt;"",Компоненты!D114,"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="E114" t="str">
         <f>IF(Компоненты!E114&lt;&gt;"",Компоненты!E114,"")</f>
-        <v/>
+        <v>6e43d176a1d591209ec3727785329eb6</v>
       </c>
       <c r="F114" t="str">
         <f>IF(Компоненты!F114&lt;&gt;"",Компоненты!F114,"")</f>
-        <v/>
+        <v>Оборудование</v>
       </c>
       <c r="G114" t="str">
         <f>IF(Компоненты!G114&lt;&gt;"",Компоненты!G114,"")</f>
-        <v/>
+        <v>Сплит-система</v>
       </c>
       <c r="H114" t="str">
         <f>IF(Компоненты!H114&lt;&gt;"",Компоненты!H114,"")</f>
@@ -18657,19 +18760,19 @@
       </c>
       <c r="I114" t="str">
         <f>IF(Компоненты!I114&lt;&gt;"",Компоненты!I114,"")</f>
-        <v/>
+        <v>Не применимо</v>
       </c>
       <c r="J114" t="str">
         <f>IF(Компоненты!J114&lt;&gt;"",Компоненты!J114,"")</f>
-        <v/>
+        <v>Базовое оборудование</v>
       </c>
       <c r="K114" t="str">
         <f>IF(Компоненты!K114&lt;&gt;"",Компоненты!K114,"")</f>
-        <v/>
+        <v>Параметрическая</v>
       </c>
       <c r="L114" t="str">
         <f>IF(Компоненты!L114&lt;&gt;"",Компоненты!L114,"")</f>
-        <v/>
+        <v>Параметризованы все габариты. Блок имеет патрубки для жидкостной и газовой линии, фреона и дренажа</v>
       </c>
       <c r="M114" t="str">
         <f>IF(Компоненты!M114&lt;&gt;"",Компоненты!M114,"")</f>
@@ -18677,15 +18780,16 @@
       </c>
       <c r="N114" t="str">
         <f>IF(Компоненты!N114&lt;&gt;"",Компоненты!N114,"")</f>
-        <v/>
+        <v>https://www.nanocad.ru/products/bim/ventilation/</v>
       </c>
       <c r="O114" t="str">
         <f>IF(Компоненты!O114&lt;&gt;"",Компоненты!O114,"")</f>
-        <v/>
+        <v>3.3…9 кВт (тепло)
+2.4…7.3 кВт (холод)</v>
       </c>
       <c r="P114" t="str">
         <f>IF(Компоненты!P114&lt;&gt;"",Компоненты!P114,"")</f>
-        <v/>
+        <v>2024.11.13</v>
       </c>
       <c r="Q114" t="str">
         <f>IF(Компоненты!Q114&lt;&gt;"",Компоненты!Q114,"")</f>
@@ -18709,29 +18813,29 @@
       </c>
     </row>
     <row r="115" spans="2:21">
-      <c r="B115" t="str">
+      <c r="B115">
         <f>IF(Компоненты!B115&lt;&gt;"",Компоненты!B115,"")</f>
-        <v/>
+        <v>112</v>
       </c>
       <c r="C115" t="str">
         <f>IF(Компоненты!C115&lt;&gt;"",Компоненты!C115,"")</f>
-        <v/>
-      </c>
-      <c r="D115" t="str">
+        <v>Сплит-система - Наружный блок</v>
+      </c>
+      <c r="D115">
         <f>IF(Компоненты!D115&lt;&gt;"",Компоненты!D115,"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="E115" t="str">
         <f>IF(Компоненты!E115&lt;&gt;"",Компоненты!E115,"")</f>
-        <v/>
+        <v>cf738be6c2382c779598f33b5432ad68</v>
       </c>
       <c r="F115" t="str">
         <f>IF(Компоненты!F115&lt;&gt;"",Компоненты!F115,"")</f>
-        <v/>
+        <v>Оборудование</v>
       </c>
       <c r="G115" t="str">
         <f>IF(Компоненты!G115&lt;&gt;"",Компоненты!G115,"")</f>
-        <v/>
+        <v>Сплит-система</v>
       </c>
       <c r="H115" t="str">
         <f>IF(Компоненты!H115&lt;&gt;"",Компоненты!H115,"")</f>
@@ -18739,19 +18843,19 @@
       </c>
       <c r="I115" t="str">
         <f>IF(Компоненты!I115&lt;&gt;"",Компоненты!I115,"")</f>
-        <v/>
+        <v>Не применимо</v>
       </c>
       <c r="J115" t="str">
         <f>IF(Компоненты!J115&lt;&gt;"",Компоненты!J115,"")</f>
-        <v/>
+        <v>Базовое оборудование</v>
       </c>
       <c r="K115" t="str">
         <f>IF(Компоненты!K115&lt;&gt;"",Компоненты!K115,"")</f>
-        <v/>
+        <v>Параметрическая</v>
       </c>
       <c r="L115" t="str">
         <f>IF(Компоненты!L115&lt;&gt;"",Компоненты!L115,"")</f>
-        <v/>
+        <v>Параметризованы все габариты. Блок имеет патрубки для жидкостной и газовой линии</v>
       </c>
       <c r="M115" t="str">
         <f>IF(Компоненты!M115&lt;&gt;"",Компоненты!M115,"")</f>
@@ -18759,15 +18863,16 @@
       </c>
       <c r="N115" t="str">
         <f>IF(Компоненты!N115&lt;&gt;"",Компоненты!N115,"")</f>
-        <v/>
+        <v>https://www.nanocad.ru/products/bim/ventilation/</v>
       </c>
       <c r="O115" t="str">
         <f>IF(Компоненты!O115&lt;&gt;"",Компоненты!O115,"")</f>
-        <v/>
+        <v>3,3…9 кВт (тепло)
+2,4…7,3 кВт (холод)</v>
       </c>
       <c r="P115" t="str">
         <f>IF(Компоненты!P115&lt;&gt;"",Компоненты!P115,"")</f>
-        <v/>
+        <v>2024.11.13</v>
       </c>
       <c r="Q115" t="str">
         <f>IF(Компоненты!Q115&lt;&gt;"",Компоненты!Q115,"")</f>

</xml_diff>

<commit_message>
VEZA New Valves & New Category Termomenters-Manometers
</commit_message>
<xml_diff>
--- a/docs/db/Base.xlsx
+++ b/docs/db/Base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\evoslib\public\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52670C72-5FBB-41FA-9492-0D838B9BB047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424E1C70-6744-4F93-B942-A0A6DE68F2EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="3492" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Параметры_компонентов" sheetId="2" r:id="rId1"/>
@@ -20,8 +20,8 @@
     <sheet name="Экспорт" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="Категория_сайта">Параметры_компонентов!$B$8:$B$16</definedName>
-    <definedName name="Категория_техническая">Параметры_компонентов!$D$8:$D$40</definedName>
+    <definedName name="Категория_сайта">Параметры_компонентов!$B$8:$B$17</definedName>
+    <definedName name="Категория_техническая">Параметры_компонентов!$D$8:$D$44</definedName>
     <definedName name="Компоненты">Таблица3[]</definedName>
     <definedName name="Название_файла">Файлы_ресурсы!$E$5:$E$24</definedName>
     <definedName name="Производитель">Параметры_компонентов!$I$8:$I$14</definedName>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1546" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1665" uniqueCount="541">
   <si>
     <t>На этом листе собраны возможные значения параметров, описывающих типы компонентов nanoCAD BIM Вентиляция</t>
   </si>
@@ -1516,9 +1516,6 @@
     <t>91...131 кВт</t>
   </si>
   <si>
-    <t>Нерпа</t>
-  </si>
-  <si>
     <t>8e67c617dc5eadaaf1db7af5048f4553</t>
   </si>
   <si>
@@ -1623,18 +1620,159 @@
   </si>
   <si>
     <t>2024.12.26</t>
+  </si>
+  <si>
+    <t>Регуляр-Л</t>
+  </si>
+  <si>
+    <t>Реглан</t>
+  </si>
+  <si>
+    <t>Клаб</t>
+  </si>
+  <si>
+    <t>Кедр-С</t>
+  </si>
+  <si>
+    <t>Гермик-Р</t>
+  </si>
+  <si>
+    <t>Гермик-П</t>
+  </si>
+  <si>
+    <t>балансировочный</t>
+  </si>
+  <si>
+    <t>регулирующий</t>
+  </si>
+  <si>
+    <t>повышенной плотности</t>
+  </si>
+  <si>
+    <t>Кедр</t>
+  </si>
+  <si>
+    <t>Все</t>
+  </si>
+  <si>
+    <t>2025.02.18</t>
+  </si>
+  <si>
+    <t>https://www.veza.ru/produktsiya/klapany-i-setevye-elementy/vozdushnye-klapany/kruglye-vozdushnye-klapany/klab-kruglyy</t>
+  </si>
+  <si>
+    <t>https://www.veza.ru/produktsiya/klapany-i-setevye-elementy/vozdushnye-klapany/pryamougolnye-vozdushnye-klapany/reglan-pryamougolnyy</t>
+  </si>
+  <si>
+    <t>https://www.veza.ru/produktsiya/klapany-i-setevye-elementy/vozdushnye-klapany/pryamougolnye-vozdushnye-klapany/regular-l-pryamougolnyy</t>
+  </si>
+  <si>
+    <t>https://www.veza.ru/produktsiya/klapany-i-setevye-elementy/vozdushnye-klapany/pryamougolnye-vozdushnye-klapany/kedr-kedr-c-pryamougolnyy</t>
+  </si>
+  <si>
+    <t>https://www.veza.ru/produktsiya/klapany-i-setevye-elementy/vozdushnye-klapany/pryamougolnye-vozdushnye-klapany/germik-p-r-c-pryamougolnyy</t>
+  </si>
+  <si>
+    <t>https://www.veza.ru/produktsiya/klapany-i-setevye-elementy/vozdushnye-klapany/kruglye-vozdushnye-klapany/nerpa-kruglyy</t>
+  </si>
+  <si>
+    <t>Нерпа, прямоугольный</t>
+  </si>
+  <si>
+    <t>Нерпа, круглый</t>
+  </si>
+  <si>
+    <t>2 версии компонента в одном *.repository:
+- с ручкой
+- с приводом ЭП.
+Параметризованы все габариты, количество приводов, автоматический подбор количества лопаток, артикул автоформируемый, защита от неправильных габаритов</t>
+  </si>
+  <si>
+    <t>2 версии компонента в одном *.repository:
+- с ручкой
+- с приводом ЭП
+Параметризованы все габариты, количество приводов, автоматический подбор количества лопаток, артикул автоформируемый, защита от неправильных габаритов</t>
+  </si>
+  <si>
+    <t>3 версии компонента в одном *.repository:
+- с ручкой
+- с приводом ЭП
+- с приводом ЭПВ
+Параметризованы все габариты, количество приводов, автоматический подбор количества лопаток, артикул автоформируемый, защита от неправильных габаритов</t>
+  </si>
+  <si>
+    <t>Манометр</t>
+  </si>
+  <si>
+    <t>Термометр</t>
+  </si>
+  <si>
+    <t>Термометры и манометры</t>
+  </si>
+  <si>
+    <t>Контрольно-измерительные приборы</t>
+  </si>
+  <si>
+    <t>Термометр с гильзой и бобышкой</t>
+  </si>
+  <si>
+    <t>Манометр с трехходовым краном и бобышкой</t>
+  </si>
+  <si>
+    <t>D40, D150</t>
+  </si>
+  <si>
+    <t>D63, D100</t>
+  </si>
+  <si>
+    <t>88f335b61cada1cfba48c53805862578</t>
+  </si>
+  <si>
+    <t>582db8a9e40bdff83e1b518f51eb4d55</t>
+  </si>
+  <si>
+    <t>dd1df4f3f072cb7c81829e19a01642ed</t>
+  </si>
+  <si>
+    <t>f205a04d42272ce6f29338099dc8a8e5</t>
+  </si>
+  <si>
+    <t>90d3e07494d941d3222cac385e9ee777</t>
+  </si>
+  <si>
+    <t>7104bb5eece4bbc9a5f6ed3ad7d0488c</t>
+  </si>
+  <si>
+    <t>991c103d429eca060e0e8be4cef9ce17</t>
+  </si>
+  <si>
+    <t>a97f7fe17eabd99172b246a30495017c</t>
+  </si>
+  <si>
+    <t>b6e48805009c9270cffaeaac90aff34c</t>
+  </si>
+  <si>
+    <t>319f3017a48f460bc38ab3a271a80a09</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1809,11 +1947,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1823,7 +1961,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1832,13 +1970,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1">
@@ -1865,13 +2003,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1880,16 +2018,19 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2542,11 +2683,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица_Привязка_категорий" displayName="Таблица_Привязка_категорий" ref="D7:E41" totalsRowCount="1">
-  <autoFilter ref="D7:E40" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D7:E40">
-    <sortCondition ref="E8:E40"/>
-    <sortCondition ref="D8:D40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица_Привязка_категорий" displayName="Таблица_Привязка_категорий" ref="D7:E45" totalsRowCount="1">
+  <autoFilter ref="D7:E44" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D7:E44">
+    <sortCondition ref="E8:E44"/>
+    <sortCondition ref="D8:D44"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Категория_техническая" totalsRowLabel="Итого"/>
@@ -2576,8 +2717,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{103355E0-29A9-421F-836A-CED6B67A811A}" name="Таблица3" displayName="Таблица3" ref="B4:V119" totalsRowShown="0" headerRowDxfId="24" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21">
-  <autoFilter ref="B4:V119" xr:uid="{103355E0-29A9-421F-836A-CED6B67A811A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{103355E0-29A9-421F-836A-CED6B67A811A}" name="Таблица3" displayName="Таблица3" ref="B4:V128" totalsRowShown="0" headerRowDxfId="24" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21">
+  <autoFilter ref="B4:V128" xr:uid="{103355E0-29A9-421F-836A-CED6B67A811A}"/>
   <tableColumns count="21">
     <tableColumn id="1" xr3:uid="{7751F2D8-B80C-49E9-82CA-3F29EFADF432}" name="id" dataDxfId="20"/>
     <tableColumn id="2" xr3:uid="{EBB32651-7529-4C31-B75F-A420D410EBF5}" name="name" dataDxfId="19"/>
@@ -2863,10 +3004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:K41"/>
+  <dimension ref="B2:K45"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -3056,7 +3197,10 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="4:5">
+    <row r="17" spans="2:5">
+      <c r="B17" t="s">
+        <v>526</v>
+      </c>
       <c r="D17" t="s">
         <v>32</v>
       </c>
@@ -3064,7 +3208,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="4:5">
+    <row r="18" spans="2:5">
       <c r="D18" t="s">
         <v>33</v>
       </c>
@@ -3072,7 +3216,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="4:5">
+    <row r="19" spans="2:5">
       <c r="D19" t="s">
         <v>34</v>
       </c>
@@ -3080,7 +3224,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="4:5">
+    <row r="20" spans="2:5">
       <c r="D20" t="s">
         <v>35</v>
       </c>
@@ -3088,7 +3232,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="4:5">
+    <row r="21" spans="2:5">
       <c r="D21" t="s">
         <v>36</v>
       </c>
@@ -3096,7 +3240,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="4:5">
+    <row r="22" spans="2:5">
       <c r="D22" t="s">
         <v>465</v>
       </c>
@@ -3104,7 +3248,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="4:5">
+    <row r="23" spans="2:5">
       <c r="D23" t="s">
         <v>458</v>
       </c>
@@ -3112,23 +3256,23 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="4:5">
+    <row r="24" spans="2:5">
       <c r="D24" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E24" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="4:5">
+    <row r="25" spans="2:5">
       <c r="D25" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E25" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="4:5">
+    <row r="26" spans="2:5">
       <c r="D26" t="s">
         <v>37</v>
       </c>
@@ -3136,7 +3280,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="4:5">
+    <row r="27" spans="2:5">
       <c r="D27" t="s">
         <v>38</v>
       </c>
@@ -3144,7 +3288,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="4:5">
+    <row r="28" spans="2:5">
       <c r="D28" t="s">
         <v>39</v>
       </c>
@@ -3152,7 +3296,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="4:5">
+    <row r="29" spans="2:5">
       <c r="D29" t="s">
         <v>40</v>
       </c>
@@ -3160,7 +3304,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="4:5">
+    <row r="30" spans="2:5">
       <c r="D30" t="s">
         <v>41</v>
       </c>
@@ -3168,7 +3312,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="4:5">
+    <row r="31" spans="2:5">
       <c r="D31" t="s">
         <v>42</v>
       </c>
@@ -3176,7 +3320,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="4:5">
+    <row r="32" spans="2:5">
       <c r="D32" t="s">
         <v>43</v>
       </c>
@@ -3240,13 +3384,29 @@
         <v>25</v>
       </c>
     </row>
+    <row r="40" spans="4:5">
+      <c r="D40" t="s">
+        <v>525</v>
+      </c>
+      <c r="E40" t="s">
+        <v>526</v>
+      </c>
+    </row>
     <row r="41" spans="4:5">
       <c r="D41" t="s">
+        <v>525</v>
+      </c>
+      <c r="E41" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="45" spans="4:5">
+      <c r="D45" t="s">
         <v>46</v>
       </c>
-      <c r="E41">
+      <c r="E45">
         <f>SUBTOTAL(103,Таблица_Привязка_категорий[Категория_сайта])</f>
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -3254,7 +3414,7 @@
     <sortCondition ref="B10"/>
   </sortState>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E40" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E44" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>Категория_сайта</formula1>
     </dataValidation>
   </dataValidations>
@@ -3857,11 +4017,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B4:V119"/>
+  <dimension ref="B4:V128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W5" sqref="W5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E126" sqref="E126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3872,11 +4032,11 @@
     <col min="5" max="5" width="18.28515625" style="4" customWidth="1"/>
     <col min="6" max="6" width="19.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="15.140625" style="1" customWidth="1"/>
     <col min="10" max="10" width="15.28515625" style="1" customWidth="1"/>
     <col min="11" max="11" width="19.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="34.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="55.85546875" style="1" customWidth="1"/>
     <col min="13" max="13" width="24.140625" style="1" customWidth="1"/>
     <col min="14" max="14" width="43.140625" style="1" customWidth="1"/>
     <col min="15" max="15" width="38.7109375" style="1" customWidth="1"/>
@@ -3965,7 +4125,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>23</v>
@@ -3987,7 +4147,7 @@
       </c>
       <c r="L5" s="11"/>
       <c r="M5" s="11" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="N5" s="17" t="s">
         <v>113</v>
@@ -3996,7 +4156,7 @@
         <v>114</v>
       </c>
       <c r="P5" s="18" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q5" s="11"/>
       <c r="R5" s="11"/>
@@ -4007,7 +4167,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="2:22" ht="105">
+    <row r="6" spans="2:22" ht="60">
       <c r="B6" s="11">
         <v>2</v>
       </c>
@@ -5657,7 +5817,7 @@
       <c r="U37" s="11"/>
       <c r="V37" s="11"/>
     </row>
-    <row r="38" spans="2:22" ht="45">
+    <row r="38" spans="2:22" ht="30">
       <c r="B38" s="11">
         <v>34</v>
       </c>
@@ -5908,7 +6068,7 @@
       <c r="U42" s="11"/>
       <c r="V42" s="11"/>
     </row>
-    <row r="43" spans="2:22" ht="60">
+    <row r="43" spans="2:22" ht="45">
       <c r="B43" s="11">
         <v>39</v>
       </c>
@@ -5959,7 +6119,7 @@
       <c r="U43" s="11"/>
       <c r="V43" s="11"/>
     </row>
-    <row r="44" spans="2:22" ht="105">
+    <row r="44" spans="2:22" ht="90">
       <c r="B44" s="11">
         <v>40</v>
       </c>
@@ -6012,7 +6172,7 @@
       <c r="U44" s="11"/>
       <c r="V44" s="11"/>
     </row>
-    <row r="45" spans="2:22" ht="90">
+    <row r="45" spans="2:22" ht="45">
       <c r="B45" s="11">
         <v>41</v>
       </c>
@@ -6175,7 +6335,7 @@
       </c>
       <c r="V47" s="11"/>
     </row>
-    <row r="48" spans="2:22" ht="45">
+    <row r="48" spans="2:22" ht="30">
       <c r="B48" s="11">
         <v>44</v>
       </c>
@@ -6230,7 +6390,7 @@
       <c r="U48" s="11"/>
       <c r="V48" s="11"/>
     </row>
-    <row r="49" spans="2:22" ht="45">
+    <row r="49" spans="2:22" ht="30">
       <c r="B49" s="11">
         <v>45</v>
       </c>
@@ -6593,7 +6753,7 @@
       <c r="U55" s="11"/>
       <c r="V55" s="11"/>
     </row>
-    <row r="56" spans="2:22" ht="60">
+    <row r="56" spans="2:22" ht="45">
       <c r="B56" s="11">
         <v>53</v>
       </c>
@@ -7755,7 +7915,7 @@
       <c r="U79" s="11"/>
       <c r="V79" s="11"/>
     </row>
-    <row r="80" spans="2:22" ht="75">
+    <row r="80" spans="2:22" ht="60">
       <c r="B80" s="11">
         <v>77</v>
       </c>
@@ -7947,7 +8107,7 @@
       <c r="U83" s="11"/>
       <c r="V83" s="11"/>
     </row>
-    <row r="84" spans="2:22" ht="75">
+    <row r="84" spans="2:22" ht="45">
       <c r="B84" s="11">
         <v>81</v>
       </c>
@@ -7994,7 +8154,7 @@
       <c r="U84" s="11"/>
       <c r="V84" s="11"/>
     </row>
-    <row r="85" spans="2:22" ht="60">
+    <row r="85" spans="2:22" ht="45">
       <c r="B85" s="11">
         <v>82</v>
       </c>
@@ -8041,7 +8201,7 @@
       <c r="U85" s="11"/>
       <c r="V85" s="11"/>
     </row>
-    <row r="86" spans="2:22" ht="90">
+    <row r="86" spans="2:22" ht="60">
       <c r="B86" s="11">
         <v>83</v>
       </c>
@@ -8135,7 +8295,7 @@
       <c r="U87" s="11"/>
       <c r="V87" s="11"/>
     </row>
-    <row r="88" spans="2:22" ht="45">
+    <row r="88" spans="2:22" ht="30">
       <c r="B88" s="11">
         <v>85</v>
       </c>
@@ -8182,7 +8342,7 @@
       <c r="U88" s="11"/>
       <c r="V88" s="11"/>
     </row>
-    <row r="89" spans="2:22" ht="60">
+    <row r="89" spans="2:22" ht="45">
       <c r="B89" s="11">
         <v>86</v>
       </c>
@@ -8333,7 +8493,7 @@
       <c r="U91" s="11"/>
       <c r="V91" s="11"/>
     </row>
-    <row r="92" spans="2:22" ht="120">
+    <row r="92" spans="2:22" ht="75">
       <c r="B92" s="11">
         <v>89</v>
       </c>
@@ -8390,7 +8550,7 @@
       <c r="U92" s="11"/>
       <c r="V92" s="11"/>
     </row>
-    <row r="93" spans="2:22" ht="120">
+    <row r="93" spans="2:22" ht="75">
       <c r="B93" s="11">
         <v>90</v>
       </c>
@@ -8447,7 +8607,7 @@
       <c r="U93" s="11"/>
       <c r="V93" s="11"/>
     </row>
-    <row r="94" spans="2:22" ht="60">
+    <row r="94" spans="2:22" ht="30">
       <c r="B94" s="11">
         <v>91</v>
       </c>
@@ -8500,7 +8660,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="95" spans="2:22" ht="60">
+    <row r="95" spans="2:22" ht="45">
       <c r="B95" s="11">
         <v>92</v>
       </c>
@@ -8653,7 +8813,7 @@
       <c r="U97" s="11"/>
       <c r="V97" s="11"/>
     </row>
-    <row r="98" spans="2:22" ht="120">
+    <row r="98" spans="2:22" ht="75">
       <c r="B98" s="11">
         <v>95</v>
       </c>
@@ -8753,7 +8913,7 @@
       <c r="U99" s="11"/>
       <c r="V99" s="11"/>
     </row>
-    <row r="100" spans="2:22" ht="225">
+    <row r="100" spans="2:22" ht="135">
       <c r="B100" s="11">
         <v>97</v>
       </c>
@@ -8804,7 +8964,7 @@
       <c r="U100" s="11"/>
       <c r="V100" s="11"/>
     </row>
-    <row r="101" spans="2:22" ht="225">
+    <row r="101" spans="2:22" ht="135">
       <c r="B101" s="11">
         <v>98</v>
       </c>
@@ -8951,7 +9111,7 @@
       <c r="U103" s="11"/>
       <c r="V103" s="11"/>
     </row>
-    <row r="104" spans="2:22" ht="60">
+    <row r="104" spans="2:22" ht="45">
       <c r="B104" s="11">
         <v>101</v>
       </c>
@@ -9055,7 +9215,7 @@
       <c r="U105" s="11"/>
       <c r="V105" s="11"/>
     </row>
-    <row r="106" spans="2:22" ht="45">
+    <row r="106" spans="2:22" ht="30">
       <c r="B106" s="11">
         <v>103</v>
       </c>
@@ -9157,7 +9317,7 @@
       <c r="U107" s="11"/>
       <c r="V107" s="11"/>
     </row>
-    <row r="108" spans="2:22" ht="60">
+    <row r="108" spans="2:22" ht="45">
       <c r="B108" s="11">
         <v>105</v>
       </c>
@@ -9259,7 +9419,7 @@
       <c r="U109" s="11"/>
       <c r="V109" s="11"/>
     </row>
-    <row r="110" spans="2:22" ht="60">
+    <row r="110" spans="2:22" ht="30">
       <c r="B110" s="11">
         <v>107</v>
       </c>
@@ -9279,7 +9439,7 @@
         <v>465</v>
       </c>
       <c r="H110" s="11" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I110" s="11" t="s">
         <v>14</v>
@@ -9310,18 +9470,18 @@
       <c r="U110" s="11"/>
       <c r="V110" s="11"/>
     </row>
-    <row r="111" spans="2:22" ht="90">
+    <row r="111" spans="2:22" ht="60">
       <c r="B111" s="11">
         <v>108</v>
       </c>
       <c r="C111" s="11" t="s">
-        <v>467</v>
+        <v>518</v>
       </c>
       <c r="D111" s="11">
         <v>1</v>
       </c>
       <c r="E111" s="13" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F111" s="11" t="s">
         <v>10</v>
@@ -9330,7 +9490,7 @@
         <v>9</v>
       </c>
       <c r="H111" s="11" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="I111" s="11" t="s">
         <v>18</v>
@@ -9342,14 +9502,14 @@
         <v>20</v>
       </c>
       <c r="L111" s="11" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="M111" s="11"/>
       <c r="N111" s="17" t="s">
+        <v>470</v>
+      </c>
+      <c r="O111" s="11" t="s">
         <v>471</v>
-      </c>
-      <c r="O111" s="11" t="s">
-        <v>472</v>
       </c>
       <c r="P111" s="18" t="s">
         <v>462</v>
@@ -9366,22 +9526,22 @@
         <v>109</v>
       </c>
       <c r="C112" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D112" s="11">
         <v>1</v>
       </c>
       <c r="E112" s="13" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F112" s="11" t="s">
         <v>29</v>
       </c>
       <c r="G112" s="11" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="H112" s="25" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="I112" s="11" t="s">
         <v>6</v>
@@ -9393,17 +9553,17 @@
         <v>20</v>
       </c>
       <c r="L112" s="11" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="M112" s="11"/>
       <c r="N112" s="17" t="s">
         <v>301</v>
       </c>
       <c r="O112" s="11" t="s">
+        <v>475</v>
+      </c>
+      <c r="P112" s="24" t="s">
         <v>476</v>
-      </c>
-      <c r="P112" s="24" t="s">
-        <v>477</v>
       </c>
       <c r="Q112" s="11"/>
       <c r="R112" s="11"/>
@@ -9417,22 +9577,22 @@
         <v>110</v>
       </c>
       <c r="C113" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D113" s="11">
         <v>1</v>
       </c>
       <c r="E113" s="13" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F113" s="11" t="s">
         <v>29</v>
       </c>
       <c r="G113" s="11" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="H113" s="25" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="I113" s="11" t="s">
         <v>6</v>
@@ -9444,17 +9604,17 @@
         <v>20</v>
       </c>
       <c r="L113" s="11" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="M113" s="11"/>
       <c r="N113" s="17" t="s">
         <v>301</v>
       </c>
       <c r="O113" s="25" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="P113" s="24" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="Q113" s="11"/>
       <c r="R113" s="11"/>
@@ -9463,24 +9623,24 @@
       <c r="U113" s="11"/>
       <c r="V113" s="11"/>
     </row>
-    <row r="114" spans="2:22" ht="60">
+    <row r="114" spans="2:22" ht="30">
       <c r="B114" s="11">
         <v>111</v>
       </c>
       <c r="C114" s="12" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D114" s="11">
         <v>1</v>
       </c>
       <c r="E114" s="13" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F114" s="11" t="s">
         <v>29</v>
       </c>
       <c r="G114" s="11" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H114" s="11"/>
       <c r="I114" s="11" t="s">
@@ -9493,17 +9653,17 @@
         <v>20</v>
       </c>
       <c r="L114" s="11" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="M114" s="11"/>
       <c r="N114" s="17" t="s">
         <v>301</v>
       </c>
       <c r="O114" s="11" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="P114" s="26" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="Q114" s="11"/>
       <c r="R114" s="11"/>
@@ -9512,24 +9672,24 @@
       <c r="U114" s="11"/>
       <c r="V114" s="11"/>
     </row>
-    <row r="115" spans="2:22" ht="45">
+    <row r="115" spans="2:22" ht="30">
       <c r="B115" s="11">
         <v>112</v>
       </c>
       <c r="C115" s="12" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D115" s="11">
         <v>1</v>
       </c>
       <c r="E115" s="13" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="F115" s="11" t="s">
         <v>29</v>
       </c>
       <c r="G115" s="11" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H115" s="11"/>
       <c r="I115" s="11" t="s">
@@ -9542,17 +9702,17 @@
         <v>20</v>
       </c>
       <c r="L115" s="11" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="M115" s="11"/>
       <c r="N115" s="17" t="s">
         <v>301</v>
       </c>
       <c r="O115" s="11" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="P115" s="26" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="Q115" s="11"/>
       <c r="R115" s="11"/>
@@ -9566,19 +9726,19 @@
         <v>113</v>
       </c>
       <c r="C116" s="11" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D116" s="11">
         <v>1</v>
       </c>
       <c r="E116" s="13" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="F116" s="11" t="s">
         <v>29</v>
       </c>
       <c r="G116" s="11" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="H116" s="11"/>
       <c r="I116" s="11" t="s">
@@ -9591,17 +9751,17 @@
         <v>20</v>
       </c>
       <c r="L116" s="11" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="M116" s="11"/>
       <c r="N116" s="17" t="s">
         <v>301</v>
       </c>
       <c r="O116" s="11" t="s">
+        <v>495</v>
+      </c>
+      <c r="P116" s="27" t="s">
         <v>496</v>
-      </c>
-      <c r="P116" s="27" t="s">
-        <v>497</v>
       </c>
       <c r="Q116" s="11"/>
       <c r="R116" s="11"/>
@@ -9610,22 +9770,50 @@
       <c r="U116" s="11"/>
       <c r="V116" s="11"/>
     </row>
-    <row r="117" spans="2:22">
-      <c r="B117" s="11"/>
-      <c r="C117" s="11"/>
-      <c r="D117" s="11"/>
-      <c r="E117" s="13"/>
-      <c r="F117" s="11"/>
-      <c r="G117" s="11"/>
-      <c r="H117" s="11"/>
-      <c r="I117" s="11"/>
-      <c r="J117" s="11"/>
-      <c r="K117" s="11"/>
-      <c r="L117" s="11"/>
+    <row r="117" spans="2:22" ht="90">
+      <c r="B117" s="11">
+        <v>114</v>
+      </c>
+      <c r="C117" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D117" s="11">
+        <v>1</v>
+      </c>
+      <c r="E117" s="13" t="s">
+        <v>531</v>
+      </c>
+      <c r="F117" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G117" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H117" s="11" t="s">
+        <v>506</v>
+      </c>
+      <c r="I117" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J117" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K117" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L117" s="11" t="s">
+        <v>520</v>
+      </c>
       <c r="M117" s="11"/>
-      <c r="N117" s="17"/>
-      <c r="O117" s="11"/>
-      <c r="P117" s="18"/>
+      <c r="N117" s="17" t="s">
+        <v>512</v>
+      </c>
+      <c r="O117" s="11" t="s">
+        <v>510</v>
+      </c>
+      <c r="P117" s="28" t="s">
+        <v>511</v>
+      </c>
       <c r="Q117" s="11"/>
       <c r="R117" s="11"/>
       <c r="S117" s="11"/>
@@ -9633,22 +9821,50 @@
       <c r="U117" s="11"/>
       <c r="V117" s="11"/>
     </row>
-    <row r="118" spans="2:22">
-      <c r="B118" s="11"/>
-      <c r="C118" s="11"/>
-      <c r="D118" s="11"/>
-      <c r="E118" s="13"/>
-      <c r="F118" s="11"/>
-      <c r="G118" s="11"/>
-      <c r="H118" s="11"/>
-      <c r="I118" s="11"/>
-      <c r="J118" s="11"/>
-      <c r="K118" s="11"/>
-      <c r="L118" s="11"/>
+    <row r="118" spans="2:22" ht="90">
+      <c r="B118" s="11">
+        <v>115</v>
+      </c>
+      <c r="C118" s="11" t="s">
+        <v>501</v>
+      </c>
+      <c r="D118" s="11">
+        <v>1</v>
+      </c>
+      <c r="E118" s="13" t="s">
+        <v>532</v>
+      </c>
+      <c r="F118" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G118" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H118" s="11" t="s">
+        <v>507</v>
+      </c>
+      <c r="I118" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J118" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K118" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L118" s="11" t="s">
+        <v>521</v>
+      </c>
       <c r="M118" s="11"/>
-      <c r="N118" s="17"/>
-      <c r="O118" s="11"/>
-      <c r="P118" s="18"/>
+      <c r="N118" s="17" t="s">
+        <v>513</v>
+      </c>
+      <c r="O118" s="11" t="s">
+        <v>510</v>
+      </c>
+      <c r="P118" s="28" t="s">
+        <v>511</v>
+      </c>
       <c r="Q118" s="11"/>
       <c r="R118" s="11"/>
       <c r="S118" s="11"/>
@@ -9656,44 +9872,463 @@
       <c r="U118" s="11"/>
       <c r="V118" s="11"/>
     </row>
-    <row r="119" spans="2:22">
-      <c r="B119" s="20"/>
-      <c r="C119" s="20"/>
-      <c r="D119" s="20"/>
-      <c r="E119" s="21"/>
-      <c r="F119" s="20"/>
-      <c r="G119" s="20"/>
-      <c r="H119" s="20"/>
-      <c r="I119" s="20"/>
-      <c r="J119" s="20"/>
-      <c r="K119" s="20"/>
-      <c r="L119" s="20"/>
-      <c r="M119" s="20"/>
-      <c r="N119" s="22"/>
-      <c r="O119" s="20"/>
-      <c r="P119" s="23"/>
-      <c r="Q119" s="20"/>
-      <c r="R119" s="20"/>
-      <c r="S119" s="20"/>
-      <c r="T119" s="20"/>
-      <c r="U119" s="20"/>
-      <c r="V119" s="20"/>
+    <row r="119" spans="2:22" ht="105">
+      <c r="B119" s="11">
+        <v>116</v>
+      </c>
+      <c r="C119" s="11" t="s">
+        <v>500</v>
+      </c>
+      <c r="D119" s="11">
+        <v>1</v>
+      </c>
+      <c r="E119" s="13" t="s">
+        <v>533</v>
+      </c>
+      <c r="F119" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G119" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H119" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="I119" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J119" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K119" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L119" s="11" t="s">
+        <v>522</v>
+      </c>
+      <c r="M119" s="11"/>
+      <c r="N119" s="17" t="s">
+        <v>514</v>
+      </c>
+      <c r="O119" s="11" t="s">
+        <v>510</v>
+      </c>
+      <c r="P119" s="28" t="s">
+        <v>511</v>
+      </c>
+      <c r="Q119" s="11"/>
+      <c r="R119" s="11"/>
+      <c r="S119" s="11"/>
+      <c r="T119" s="11"/>
+      <c r="U119" s="11"/>
+      <c r="V119" s="11"/>
+    </row>
+    <row r="120" spans="2:22" ht="105">
+      <c r="B120" s="11">
+        <v>117</v>
+      </c>
+      <c r="C120" s="11" t="s">
+        <v>509</v>
+      </c>
+      <c r="D120" s="11">
+        <v>1</v>
+      </c>
+      <c r="E120" s="13" t="s">
+        <v>534</v>
+      </c>
+      <c r="F120" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G120" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H120" s="11" t="s">
+        <v>508</v>
+      </c>
+      <c r="I120" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J120" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K120" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L120" s="11" t="s">
+        <v>522</v>
+      </c>
+      <c r="M120" s="11"/>
+      <c r="N120" s="17" t="s">
+        <v>515</v>
+      </c>
+      <c r="O120" s="11" t="s">
+        <v>510</v>
+      </c>
+      <c r="P120" s="28" t="s">
+        <v>511</v>
+      </c>
+      <c r="Q120" s="11"/>
+      <c r="R120" s="11"/>
+      <c r="S120" s="11"/>
+      <c r="T120" s="11"/>
+      <c r="U120" s="11"/>
+      <c r="V120" s="11"/>
+    </row>
+    <row r="121" spans="2:22" ht="105">
+      <c r="B121" s="11">
+        <v>118</v>
+      </c>
+      <c r="C121" s="11" t="s">
+        <v>503</v>
+      </c>
+      <c r="D121" s="11">
+        <v>1</v>
+      </c>
+      <c r="E121" s="13" t="s">
+        <v>535</v>
+      </c>
+      <c r="F121" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G121" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H121" s="11" t="s">
+        <v>508</v>
+      </c>
+      <c r="I121" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J121" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K121" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L121" s="11" t="s">
+        <v>522</v>
+      </c>
+      <c r="M121" s="11"/>
+      <c r="N121" s="17" t="s">
+        <v>515</v>
+      </c>
+      <c r="O121" s="11" t="s">
+        <v>510</v>
+      </c>
+      <c r="P121" s="28" t="s">
+        <v>511</v>
+      </c>
+      <c r="Q121" s="11"/>
+      <c r="R121" s="11"/>
+      <c r="S121" s="11"/>
+      <c r="T121" s="11"/>
+      <c r="U121" s="11"/>
+      <c r="V121" s="11"/>
+    </row>
+    <row r="122" spans="2:22" ht="105">
+      <c r="B122" s="11">
+        <v>119</v>
+      </c>
+      <c r="C122" s="11" t="s">
+        <v>504</v>
+      </c>
+      <c r="D122" s="11">
+        <v>1</v>
+      </c>
+      <c r="E122" s="13" t="s">
+        <v>536</v>
+      </c>
+      <c r="F122" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G122" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H122" s="11"/>
+      <c r="I122" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J122" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K122" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L122" s="11" t="s">
+        <v>522</v>
+      </c>
+      <c r="M122" s="11"/>
+      <c r="N122" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="O122" s="11" t="s">
+        <v>510</v>
+      </c>
+      <c r="P122" s="28" t="s">
+        <v>511</v>
+      </c>
+      <c r="Q122" s="11"/>
+      <c r="R122" s="11"/>
+      <c r="S122" s="11"/>
+      <c r="T122" s="11"/>
+      <c r="U122" s="11"/>
+      <c r="V122" s="11"/>
+    </row>
+    <row r="123" spans="2:22" ht="105">
+      <c r="B123" s="11">
+        <v>120</v>
+      </c>
+      <c r="C123" s="11" t="s">
+        <v>505</v>
+      </c>
+      <c r="D123" s="11">
+        <v>1</v>
+      </c>
+      <c r="E123" s="13" t="s">
+        <v>537</v>
+      </c>
+      <c r="F123" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G123" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H123" s="11"/>
+      <c r="I123" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J123" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K123" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L123" s="11" t="s">
+        <v>522</v>
+      </c>
+      <c r="M123" s="11"/>
+      <c r="N123" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="O123" s="11" t="s">
+        <v>510</v>
+      </c>
+      <c r="P123" s="28" t="s">
+        <v>511</v>
+      </c>
+      <c r="Q123" s="11"/>
+      <c r="R123" s="11"/>
+      <c r="S123" s="11"/>
+      <c r="T123" s="11"/>
+      <c r="U123" s="11"/>
+      <c r="V123" s="11"/>
+    </row>
+    <row r="124" spans="2:22" ht="105">
+      <c r="B124" s="11">
+        <v>121</v>
+      </c>
+      <c r="C124" s="11" t="s">
+        <v>519</v>
+      </c>
+      <c r="D124" s="11">
+        <v>1</v>
+      </c>
+      <c r="E124" s="13" t="s">
+        <v>538</v>
+      </c>
+      <c r="F124" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G124" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H124" s="11" t="s">
+        <v>468</v>
+      </c>
+      <c r="I124" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J124" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K124" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L124" s="11" t="s">
+        <v>522</v>
+      </c>
+      <c r="M124" s="11"/>
+      <c r="N124" s="17" t="s">
+        <v>517</v>
+      </c>
+      <c r="O124" s="11" t="s">
+        <v>510</v>
+      </c>
+      <c r="P124" s="28" t="s">
+        <v>511</v>
+      </c>
+      <c r="Q124" s="11"/>
+      <c r="R124" s="11"/>
+      <c r="S124" s="11"/>
+      <c r="T124" s="11"/>
+      <c r="U124" s="11"/>
+      <c r="V124" s="11"/>
+    </row>
+    <row r="125" spans="2:22" ht="45">
+      <c r="B125" s="11">
+        <v>122</v>
+      </c>
+      <c r="C125" s="11" t="s">
+        <v>523</v>
+      </c>
+      <c r="D125" s="11">
+        <v>1</v>
+      </c>
+      <c r="E125" s="13" t="s">
+        <v>539</v>
+      </c>
+      <c r="F125" s="11" t="s">
+        <v>526</v>
+      </c>
+      <c r="G125" s="11" t="s">
+        <v>525</v>
+      </c>
+      <c r="H125" s="11"/>
+      <c r="I125" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="J125" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K125" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L125" s="11" t="s">
+        <v>527</v>
+      </c>
+      <c r="M125" s="11"/>
+      <c r="N125" s="17"/>
+      <c r="O125" s="11" t="s">
+        <v>530</v>
+      </c>
+      <c r="P125" s="28" t="s">
+        <v>511</v>
+      </c>
+      <c r="Q125" s="11"/>
+      <c r="R125" s="11"/>
+      <c r="S125" s="11"/>
+      <c r="T125" s="11"/>
+      <c r="U125" s="11"/>
+      <c r="V125" s="11"/>
+    </row>
+    <row r="126" spans="2:22" ht="45">
+      <c r="B126" s="11">
+        <v>123</v>
+      </c>
+      <c r="C126" s="11" t="s">
+        <v>524</v>
+      </c>
+      <c r="D126" s="11">
+        <v>1</v>
+      </c>
+      <c r="E126" s="13" t="s">
+        <v>540</v>
+      </c>
+      <c r="F126" s="11" t="s">
+        <v>526</v>
+      </c>
+      <c r="G126" s="11" t="s">
+        <v>525</v>
+      </c>
+      <c r="H126" s="11"/>
+      <c r="I126" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="J126" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K126" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L126" s="11" t="s">
+        <v>528</v>
+      </c>
+      <c r="M126" s="11"/>
+      <c r="N126" s="17"/>
+      <c r="O126" s="11" t="s">
+        <v>529</v>
+      </c>
+      <c r="P126" s="28" t="s">
+        <v>511</v>
+      </c>
+      <c r="Q126" s="11"/>
+      <c r="R126" s="11"/>
+      <c r="S126" s="11"/>
+      <c r="T126" s="11"/>
+      <c r="U126" s="11"/>
+      <c r="V126" s="11"/>
+    </row>
+    <row r="127" spans="2:22">
+      <c r="B127" s="11"/>
+      <c r="C127" s="11"/>
+      <c r="D127" s="11"/>
+      <c r="E127" s="13"/>
+      <c r="F127" s="11"/>
+      <c r="G127" s="11"/>
+      <c r="H127" s="11"/>
+      <c r="I127" s="11"/>
+      <c r="J127" s="11"/>
+      <c r="K127" s="11"/>
+      <c r="L127" s="11"/>
+      <c r="M127" s="11"/>
+      <c r="N127" s="17"/>
+      <c r="O127" s="11"/>
+      <c r="P127" s="18"/>
+      <c r="Q127" s="11"/>
+      <c r="R127" s="11"/>
+      <c r="S127" s="11"/>
+      <c r="T127" s="11"/>
+      <c r="U127" s="11"/>
+      <c r="V127" s="11"/>
+    </row>
+    <row r="128" spans="2:22">
+      <c r="B128" s="20"/>
+      <c r="C128" s="20"/>
+      <c r="D128" s="20"/>
+      <c r="E128" s="21"/>
+      <c r="F128" s="20"/>
+      <c r="G128" s="20"/>
+      <c r="H128" s="20"/>
+      <c r="I128" s="20"/>
+      <c r="J128" s="20"/>
+      <c r="K128" s="20"/>
+      <c r="L128" s="20"/>
+      <c r="M128" s="20"/>
+      <c r="N128" s="22"/>
+      <c r="O128" s="20"/>
+      <c r="P128" s="23"/>
+      <c r="Q128" s="20"/>
+      <c r="R128" s="20"/>
+      <c r="S128" s="20"/>
+      <c r="T128" s="20"/>
+      <c r="U128" s="20"/>
+      <c r="V128" s="20"/>
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F119" xr:uid="{CA629B07-12E3-4B2C-BDDB-FADC282D102C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F128" xr:uid="{CA629B07-12E3-4B2C-BDDB-FADC282D102C}">
       <formula1>Категория_сайта</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G119" xr:uid="{B6344CF3-F6AF-41DB-8994-C9864C10B114}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G128" xr:uid="{B6344CF3-F6AF-41DB-8994-C9864C10B114}">
       <formula1>Категория_техническая</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I119" xr:uid="{F86BF9AC-9A89-4F9F-8C41-D243F4D941A3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I128" xr:uid="{F86BF9AC-9A89-4F9F-8C41-D243F4D941A3}">
       <formula1>Форма</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J119" xr:uid="{5F113A00-85DF-4893-889F-77AB208671C5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J128" xr:uid="{5F113A00-85DF-4893-889F-77AB208671C5}">
       <formula1>Производитель</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5:K119" xr:uid="{7151652D-EAD3-4C3E-B748-514F3AB46DEB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5:K128" xr:uid="{7151652D-EAD3-4C3E-B748-514F3AB46DEB}">
       <formula1>Тип_графики</formula1>
     </dataValidation>
   </dataValidations>
@@ -9709,8 +10344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B4:U200"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="C119" sqref="C119"/>
+    <sheetView topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="F117" sqref="F117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -18544,7 +19179,7 @@
       </c>
       <c r="C111" t="str">
         <f>IF(Компоненты!C111&lt;&gt;"",Компоненты!C111,"")</f>
-        <v>Нерпа</v>
+        <v>Нерпа, прямоугольный</v>
       </c>
       <c r="D111">
         <f>IF(Компоненты!D111&lt;&gt;"",Компоненты!D111,"")</f>
@@ -19037,49 +19672,52 @@
       </c>
     </row>
     <row r="117" spans="2:21">
-      <c r="B117" t="str">
+      <c r="B117">
         <f>IF(Компоненты!B117&lt;&gt;"",Компоненты!B117,"")</f>
-        <v/>
+        <v>114</v>
       </c>
       <c r="C117" t="str">
         <f>IF(Компоненты!C117&lt;&gt;"",Компоненты!C117,"")</f>
-        <v/>
-      </c>
-      <c r="D117" t="str">
+        <v>Клаб</v>
+      </c>
+      <c r="D117">
         <f>IF(Компоненты!D117&lt;&gt;"",Компоненты!D117,"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="E117" t="str">
         <f>IF(Компоненты!E117&lt;&gt;"",Компоненты!E117,"")</f>
-        <v/>
+        <v>88f335b61cada1cfba48c53805862578</v>
       </c>
       <c r="F117" t="str">
         <f>IF(Компоненты!F117&lt;&gt;"",Компоненты!F117,"")</f>
-        <v/>
+        <v>Арматура воздуховодов</v>
       </c>
       <c r="G117" t="str">
         <f>IF(Компоненты!G117&lt;&gt;"",Компоненты!G117,"")</f>
-        <v/>
+        <v>Клапан воздушный</v>
       </c>
       <c r="H117" t="str">
         <f>IF(Компоненты!H117&lt;&gt;"",Компоненты!H117,"")</f>
-        <v/>
+        <v>балансировочный</v>
       </c>
       <c r="I117" t="str">
         <f>IF(Компоненты!I117&lt;&gt;"",Компоненты!I117,"")</f>
-        <v/>
+        <v>Круглый</v>
       </c>
       <c r="J117" t="str">
         <f>IF(Компоненты!J117&lt;&gt;"",Компоненты!J117,"")</f>
-        <v/>
+        <v>Веза</v>
       </c>
       <c r="K117" t="str">
         <f>IF(Компоненты!K117&lt;&gt;"",Компоненты!K117,"")</f>
-        <v/>
+        <v>Параметрическая</v>
       </c>
       <c r="L117" t="str">
         <f>IF(Компоненты!L117&lt;&gt;"",Компоненты!L117,"")</f>
-        <v/>
+        <v>2 версии компонента в одном *.repository:
+- с ручкой
+- с приводом ЭП.
+Параметризованы все габариты, количество приводов, автоматический подбор количества лопаток, артикул автоформируемый, защита от неправильных габаритов</v>
       </c>
       <c r="M117" t="str">
         <f>IF(Компоненты!M117&lt;&gt;"",Компоненты!M117,"")</f>
@@ -19087,15 +19725,15 @@
       </c>
       <c r="N117" t="str">
         <f>IF(Компоненты!N117&lt;&gt;"",Компоненты!N117,"")</f>
-        <v/>
+        <v>https://www.veza.ru/produktsiya/klapany-i-setevye-elementy/vozdushnye-klapany/kruglye-vozdushnye-klapany/klab-kruglyy</v>
       </c>
       <c r="O117" t="str">
         <f>IF(Компоненты!O117&lt;&gt;"",Компоненты!O117,"")</f>
-        <v/>
+        <v>Все</v>
       </c>
       <c r="P117" t="str">
         <f>IF(Компоненты!P117&lt;&gt;"",Компоненты!P117,"")</f>
-        <v/>
+        <v>2025.02.18</v>
       </c>
       <c r="Q117" t="str">
         <f>IF(Компоненты!Q117&lt;&gt;"",Компоненты!Q117,"")</f>
@@ -19119,49 +19757,52 @@
       </c>
     </row>
     <row r="118" spans="2:21">
-      <c r="B118" t="str">
+      <c r="B118">
         <f>IF(Компоненты!B118&lt;&gt;"",Компоненты!B118,"")</f>
-        <v/>
+        <v>115</v>
       </c>
       <c r="C118" t="str">
         <f>IF(Компоненты!C118&lt;&gt;"",Компоненты!C118,"")</f>
-        <v/>
-      </c>
-      <c r="D118" t="str">
+        <v>Реглан</v>
+      </c>
+      <c r="D118">
         <f>IF(Компоненты!D118&lt;&gt;"",Компоненты!D118,"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="E118" t="str">
         <f>IF(Компоненты!E118&lt;&gt;"",Компоненты!E118,"")</f>
-        <v/>
+        <v>582db8a9e40bdff83e1b518f51eb4d55</v>
       </c>
       <c r="F118" t="str">
         <f>IF(Компоненты!F118&lt;&gt;"",Компоненты!F118,"")</f>
-        <v/>
+        <v>Арматура воздуховодов</v>
       </c>
       <c r="G118" t="str">
         <f>IF(Компоненты!G118&lt;&gt;"",Компоненты!G118,"")</f>
-        <v/>
+        <v>Клапан воздушный</v>
       </c>
       <c r="H118" t="str">
         <f>IF(Компоненты!H118&lt;&gt;"",Компоненты!H118,"")</f>
-        <v/>
+        <v>регулирующий</v>
       </c>
       <c r="I118" t="str">
         <f>IF(Компоненты!I118&lt;&gt;"",Компоненты!I118,"")</f>
-        <v/>
+        <v>Прямоугольный</v>
       </c>
       <c r="J118" t="str">
         <f>IF(Компоненты!J118&lt;&gt;"",Компоненты!J118,"")</f>
-        <v/>
+        <v>Веза</v>
       </c>
       <c r="K118" t="str">
         <f>IF(Компоненты!K118&lt;&gt;"",Компоненты!K118,"")</f>
-        <v/>
+        <v>Параметрическая</v>
       </c>
       <c r="L118" t="str">
         <f>IF(Компоненты!L118&lt;&gt;"",Компоненты!L118,"")</f>
-        <v/>
+        <v>2 версии компонента в одном *.repository:
+- с ручкой
+- с приводом ЭП
+Параметризованы все габариты, количество приводов, автоматический подбор количества лопаток, артикул автоформируемый, защита от неправильных габаритов</v>
       </c>
       <c r="M118" t="str">
         <f>IF(Компоненты!M118&lt;&gt;"",Компоненты!M118,"")</f>
@@ -19169,15 +19810,15 @@
       </c>
       <c r="N118" t="str">
         <f>IF(Компоненты!N118&lt;&gt;"",Компоненты!N118,"")</f>
-        <v/>
+        <v>https://www.veza.ru/produktsiya/klapany-i-setevye-elementy/vozdushnye-klapany/pryamougolnye-vozdushnye-klapany/reglan-pryamougolnyy</v>
       </c>
       <c r="O118" t="str">
         <f>IF(Компоненты!O118&lt;&gt;"",Компоненты!O118,"")</f>
-        <v/>
+        <v>Все</v>
       </c>
       <c r="P118" t="str">
         <f>IF(Компоненты!P118&lt;&gt;"",Компоненты!P118,"")</f>
-        <v/>
+        <v>2025.02.18</v>
       </c>
       <c r="Q118" t="str">
         <f>IF(Компоненты!Q118&lt;&gt;"",Компоненты!Q118,"")</f>
@@ -19201,49 +19842,53 @@
       </c>
     </row>
     <row r="119" spans="2:21">
-      <c r="B119" t="str">
+      <c r="B119">
         <f>IF(Компоненты!B119&lt;&gt;"",Компоненты!B119,"")</f>
-        <v/>
+        <v>116</v>
       </c>
       <c r="C119" t="str">
         <f>IF(Компоненты!C119&lt;&gt;"",Компоненты!C119,"")</f>
-        <v/>
-      </c>
-      <c r="D119" t="str">
+        <v>Регуляр-Л</v>
+      </c>
+      <c r="D119">
         <f>IF(Компоненты!D119&lt;&gt;"",Компоненты!D119,"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="E119" t="str">
         <f>IF(Компоненты!E119&lt;&gt;"",Компоненты!E119,"")</f>
-        <v/>
+        <v>dd1df4f3f072cb7c81829e19a01642ed</v>
       </c>
       <c r="F119" t="str">
         <f>IF(Компоненты!F119&lt;&gt;"",Компоненты!F119,"")</f>
-        <v/>
+        <v>Арматура воздуховодов</v>
       </c>
       <c r="G119" t="str">
         <f>IF(Компоненты!G119&lt;&gt;"",Компоненты!G119,"")</f>
-        <v/>
+        <v>Клапан воздушный</v>
       </c>
       <c r="H119" t="str">
         <f>IF(Компоненты!H119&lt;&gt;"",Компоненты!H119,"")</f>
-        <v/>
+        <v>универсальный</v>
       </c>
       <c r="I119" t="str">
         <f>IF(Компоненты!I119&lt;&gt;"",Компоненты!I119,"")</f>
-        <v/>
+        <v>Прямоугольный</v>
       </c>
       <c r="J119" t="str">
         <f>IF(Компоненты!J119&lt;&gt;"",Компоненты!J119,"")</f>
-        <v/>
+        <v>Веза</v>
       </c>
       <c r="K119" t="str">
         <f>IF(Компоненты!K119&lt;&gt;"",Компоненты!K119,"")</f>
-        <v/>
+        <v>Параметрическая</v>
       </c>
       <c r="L119" t="str">
         <f>IF(Компоненты!L119&lt;&gt;"",Компоненты!L119,"")</f>
-        <v/>
+        <v>3 версии компонента в одном *.repository:
+- с ручкой
+- с приводом ЭП
+- с приводом ЭПВ
+Параметризованы все габариты, количество приводов, автоматический подбор количества лопаток, артикул автоформируемый, защита от неправильных габаритов</v>
       </c>
       <c r="M119" t="str">
         <f>IF(Компоненты!M119&lt;&gt;"",Компоненты!M119,"")</f>
@@ -19251,15 +19896,15 @@
       </c>
       <c r="N119" t="str">
         <f>IF(Компоненты!N119&lt;&gt;"",Компоненты!N119,"")</f>
-        <v/>
+        <v>https://www.veza.ru/produktsiya/klapany-i-setevye-elementy/vozdushnye-klapany/pryamougolnye-vozdushnye-klapany/regular-l-pryamougolnyy</v>
       </c>
       <c r="O119" t="str">
         <f>IF(Компоненты!O119&lt;&gt;"",Компоненты!O119,"")</f>
-        <v/>
+        <v>Все</v>
       </c>
       <c r="P119" t="str">
         <f>IF(Компоненты!P119&lt;&gt;"",Компоненты!P119,"")</f>
-        <v/>
+        <v>2025.02.18</v>
       </c>
       <c r="Q119" t="str">
         <f>IF(Компоненты!Q119&lt;&gt;"",Компоненты!Q119,"")</f>
@@ -19283,49 +19928,53 @@
       </c>
     </row>
     <row r="120" spans="2:21">
-      <c r="B120" t="str">
+      <c r="B120">
         <f>IF(Компоненты!B120&lt;&gt;"",Компоненты!B120,"")</f>
-        <v/>
+        <v>117</v>
       </c>
       <c r="C120" t="str">
         <f>IF(Компоненты!C120&lt;&gt;"",Компоненты!C120,"")</f>
-        <v/>
-      </c>
-      <c r="D120" t="str">
+        <v>Кедр</v>
+      </c>
+      <c r="D120">
         <f>IF(Компоненты!D120&lt;&gt;"",Компоненты!D120,"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="E120" t="str">
         <f>IF(Компоненты!E120&lt;&gt;"",Компоненты!E120,"")</f>
-        <v/>
+        <v>f205a04d42272ce6f29338099dc8a8e5</v>
       </c>
       <c r="F120" t="str">
         <f>IF(Компоненты!F120&lt;&gt;"",Компоненты!F120,"")</f>
-        <v/>
+        <v>Арматура воздуховодов</v>
       </c>
       <c r="G120" t="str">
         <f>IF(Компоненты!G120&lt;&gt;"",Компоненты!G120,"")</f>
-        <v/>
+        <v>Клапан воздушный</v>
       </c>
       <c r="H120" t="str">
         <f>IF(Компоненты!H120&lt;&gt;"",Компоненты!H120,"")</f>
-        <v/>
+        <v>повышенной плотности</v>
       </c>
       <c r="I120" t="str">
         <f>IF(Компоненты!I120&lt;&gt;"",Компоненты!I120,"")</f>
-        <v/>
+        <v>Прямоугольный</v>
       </c>
       <c r="J120" t="str">
         <f>IF(Компоненты!J120&lt;&gt;"",Компоненты!J120,"")</f>
-        <v/>
+        <v>Веза</v>
       </c>
       <c r="K120" t="str">
         <f>IF(Компоненты!K120&lt;&gt;"",Компоненты!K120,"")</f>
-        <v/>
+        <v>Параметрическая</v>
       </c>
       <c r="L120" t="str">
         <f>IF(Компоненты!L120&lt;&gt;"",Компоненты!L120,"")</f>
-        <v/>
+        <v>3 версии компонента в одном *.repository:
+- с ручкой
+- с приводом ЭП
+- с приводом ЭПВ
+Параметризованы все габариты, количество приводов, автоматический подбор количества лопаток, артикул автоформируемый, защита от неправильных габаритов</v>
       </c>
       <c r="M120" t="str">
         <f>IF(Компоненты!M120&lt;&gt;"",Компоненты!M120,"")</f>
@@ -19333,15 +19982,15 @@
       </c>
       <c r="N120" t="str">
         <f>IF(Компоненты!N120&lt;&gt;"",Компоненты!N120,"")</f>
-        <v/>
+        <v>https://www.veza.ru/produktsiya/klapany-i-setevye-elementy/vozdushnye-klapany/pryamougolnye-vozdushnye-klapany/kedr-kedr-c-pryamougolnyy</v>
       </c>
       <c r="O120" t="str">
         <f>IF(Компоненты!O120&lt;&gt;"",Компоненты!O120,"")</f>
-        <v/>
+        <v>Все</v>
       </c>
       <c r="P120" t="str">
         <f>IF(Компоненты!P120&lt;&gt;"",Компоненты!P120,"")</f>
-        <v/>
+        <v>2025.02.18</v>
       </c>
       <c r="Q120" t="str">
         <f>IF(Компоненты!Q120&lt;&gt;"",Компоненты!Q120,"")</f>
@@ -19365,49 +20014,53 @@
       </c>
     </row>
     <row r="121" spans="2:21">
-      <c r="B121" t="str">
+      <c r="B121">
         <f>IF(Компоненты!B121&lt;&gt;"",Компоненты!B121,"")</f>
-        <v/>
+        <v>118</v>
       </c>
       <c r="C121" t="str">
         <f>IF(Компоненты!C121&lt;&gt;"",Компоненты!C121,"")</f>
-        <v/>
-      </c>
-      <c r="D121" t="str">
+        <v>Кедр-С</v>
+      </c>
+      <c r="D121">
         <f>IF(Компоненты!D121&lt;&gt;"",Компоненты!D121,"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="E121" t="str">
         <f>IF(Компоненты!E121&lt;&gt;"",Компоненты!E121,"")</f>
-        <v/>
+        <v>90d3e07494d941d3222cac385e9ee777</v>
       </c>
       <c r="F121" t="str">
         <f>IF(Компоненты!F121&lt;&gt;"",Компоненты!F121,"")</f>
-        <v/>
+        <v>Арматура воздуховодов</v>
       </c>
       <c r="G121" t="str">
         <f>IF(Компоненты!G121&lt;&gt;"",Компоненты!G121,"")</f>
-        <v/>
+        <v>Клапан воздушный</v>
       </c>
       <c r="H121" t="str">
         <f>IF(Компоненты!H121&lt;&gt;"",Компоненты!H121,"")</f>
-        <v/>
+        <v>повышенной плотности</v>
       </c>
       <c r="I121" t="str">
         <f>IF(Компоненты!I121&lt;&gt;"",Компоненты!I121,"")</f>
-        <v/>
+        <v>Прямоугольный</v>
       </c>
       <c r="J121" t="str">
         <f>IF(Компоненты!J121&lt;&gt;"",Компоненты!J121,"")</f>
-        <v/>
+        <v>Веза</v>
       </c>
       <c r="K121" t="str">
         <f>IF(Компоненты!K121&lt;&gt;"",Компоненты!K121,"")</f>
-        <v/>
+        <v>Параметрическая</v>
       </c>
       <c r="L121" t="str">
         <f>IF(Компоненты!L121&lt;&gt;"",Компоненты!L121,"")</f>
-        <v/>
+        <v>3 версии компонента в одном *.repository:
+- с ручкой
+- с приводом ЭП
+- с приводом ЭПВ
+Параметризованы все габариты, количество приводов, автоматический подбор количества лопаток, артикул автоформируемый, защита от неправильных габаритов</v>
       </c>
       <c r="M121" t="str">
         <f>IF(Компоненты!M121&lt;&gt;"",Компоненты!M121,"")</f>
@@ -19415,15 +20068,15 @@
       </c>
       <c r="N121" t="str">
         <f>IF(Компоненты!N121&lt;&gt;"",Компоненты!N121,"")</f>
-        <v/>
+        <v>https://www.veza.ru/produktsiya/klapany-i-setevye-elementy/vozdushnye-klapany/pryamougolnye-vozdushnye-klapany/kedr-kedr-c-pryamougolnyy</v>
       </c>
       <c r="O121" t="str">
         <f>IF(Компоненты!O121&lt;&gt;"",Компоненты!O121,"")</f>
-        <v/>
+        <v>Все</v>
       </c>
       <c r="P121" t="str">
         <f>IF(Компоненты!P121&lt;&gt;"",Компоненты!P121,"")</f>
-        <v/>
+        <v>2025.02.18</v>
       </c>
       <c r="Q121" t="str">
         <f>IF(Компоненты!Q121&lt;&gt;"",Компоненты!Q121,"")</f>
@@ -19447,29 +20100,29 @@
       </c>
     </row>
     <row r="122" spans="2:21">
-      <c r="B122" t="str">
+      <c r="B122">
         <f>IF(Компоненты!B122&lt;&gt;"",Компоненты!B122,"")</f>
-        <v/>
+        <v>119</v>
       </c>
       <c r="C122" t="str">
         <f>IF(Компоненты!C122&lt;&gt;"",Компоненты!C122,"")</f>
-        <v/>
-      </c>
-      <c r="D122" t="str">
+        <v>Гермик-Р</v>
+      </c>
+      <c r="D122">
         <f>IF(Компоненты!D122&lt;&gt;"",Компоненты!D122,"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="E122" t="str">
         <f>IF(Компоненты!E122&lt;&gt;"",Компоненты!E122,"")</f>
-        <v/>
+        <v>7104bb5eece4bbc9a5f6ed3ad7d0488c</v>
       </c>
       <c r="F122" t="str">
         <f>IF(Компоненты!F122&lt;&gt;"",Компоненты!F122,"")</f>
-        <v/>
+        <v>Арматура воздуховодов</v>
       </c>
       <c r="G122" t="str">
         <f>IF(Компоненты!G122&lt;&gt;"",Компоненты!G122,"")</f>
-        <v/>
+        <v>Клапан воздушный</v>
       </c>
       <c r="H122" t="str">
         <f>IF(Компоненты!H122&lt;&gt;"",Компоненты!H122,"")</f>
@@ -19477,19 +20130,23 @@
       </c>
       <c r="I122" t="str">
         <f>IF(Компоненты!I122&lt;&gt;"",Компоненты!I122,"")</f>
-        <v/>
+        <v>Прямоугольный</v>
       </c>
       <c r="J122" t="str">
         <f>IF(Компоненты!J122&lt;&gt;"",Компоненты!J122,"")</f>
-        <v/>
+        <v>Веза</v>
       </c>
       <c r="K122" t="str">
         <f>IF(Компоненты!K122&lt;&gt;"",Компоненты!K122,"")</f>
-        <v/>
+        <v>Параметрическая</v>
       </c>
       <c r="L122" t="str">
         <f>IF(Компоненты!L122&lt;&gt;"",Компоненты!L122,"")</f>
-        <v/>
+        <v>3 версии компонента в одном *.repository:
+- с ручкой
+- с приводом ЭП
+- с приводом ЭПВ
+Параметризованы все габариты, количество приводов, автоматический подбор количества лопаток, артикул автоформируемый, защита от неправильных габаритов</v>
       </c>
       <c r="M122" t="str">
         <f>IF(Компоненты!M122&lt;&gt;"",Компоненты!M122,"")</f>
@@ -19497,15 +20154,15 @@
       </c>
       <c r="N122" t="str">
         <f>IF(Компоненты!N122&lt;&gt;"",Компоненты!N122,"")</f>
-        <v/>
+        <v>https://www.veza.ru/produktsiya/klapany-i-setevye-elementy/vozdushnye-klapany/pryamougolnye-vozdushnye-klapany/germik-p-r-c-pryamougolnyy</v>
       </c>
       <c r="O122" t="str">
         <f>IF(Компоненты!O122&lt;&gt;"",Компоненты!O122,"")</f>
-        <v/>
+        <v>Все</v>
       </c>
       <c r="P122" t="str">
         <f>IF(Компоненты!P122&lt;&gt;"",Компоненты!P122,"")</f>
-        <v/>
+        <v>2025.02.18</v>
       </c>
       <c r="Q122" t="str">
         <f>IF(Компоненты!Q122&lt;&gt;"",Компоненты!Q122,"")</f>
@@ -19529,29 +20186,29 @@
       </c>
     </row>
     <row r="123" spans="2:21">
-      <c r="B123" t="str">
+      <c r="B123">
         <f>IF(Компоненты!B123&lt;&gt;"",Компоненты!B123,"")</f>
-        <v/>
+        <v>120</v>
       </c>
       <c r="C123" t="str">
         <f>IF(Компоненты!C123&lt;&gt;"",Компоненты!C123,"")</f>
-        <v/>
-      </c>
-      <c r="D123" t="str">
+        <v>Гермик-П</v>
+      </c>
+      <c r="D123">
         <f>IF(Компоненты!D123&lt;&gt;"",Компоненты!D123,"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="E123" t="str">
         <f>IF(Компоненты!E123&lt;&gt;"",Компоненты!E123,"")</f>
-        <v/>
+        <v>991c103d429eca060e0e8be4cef9ce17</v>
       </c>
       <c r="F123" t="str">
         <f>IF(Компоненты!F123&lt;&gt;"",Компоненты!F123,"")</f>
-        <v/>
+        <v>Арматура воздуховодов</v>
       </c>
       <c r="G123" t="str">
         <f>IF(Компоненты!G123&lt;&gt;"",Компоненты!G123,"")</f>
-        <v/>
+        <v>Клапан воздушный</v>
       </c>
       <c r="H123" t="str">
         <f>IF(Компоненты!H123&lt;&gt;"",Компоненты!H123,"")</f>
@@ -19559,19 +20216,23 @@
       </c>
       <c r="I123" t="str">
         <f>IF(Компоненты!I123&lt;&gt;"",Компоненты!I123,"")</f>
-        <v/>
+        <v>Прямоугольный</v>
       </c>
       <c r="J123" t="str">
         <f>IF(Компоненты!J123&lt;&gt;"",Компоненты!J123,"")</f>
-        <v/>
+        <v>Веза</v>
       </c>
       <c r="K123" t="str">
         <f>IF(Компоненты!K123&lt;&gt;"",Компоненты!K123,"")</f>
-        <v/>
+        <v>Параметрическая</v>
       </c>
       <c r="L123" t="str">
         <f>IF(Компоненты!L123&lt;&gt;"",Компоненты!L123,"")</f>
-        <v/>
+        <v>3 версии компонента в одном *.repository:
+- с ручкой
+- с приводом ЭП
+- с приводом ЭПВ
+Параметризованы все габариты, количество приводов, автоматический подбор количества лопаток, артикул автоформируемый, защита от неправильных габаритов</v>
       </c>
       <c r="M123" t="str">
         <f>IF(Компоненты!M123&lt;&gt;"",Компоненты!M123,"")</f>
@@ -19579,15 +20240,15 @@
       </c>
       <c r="N123" t="str">
         <f>IF(Компоненты!N123&lt;&gt;"",Компоненты!N123,"")</f>
-        <v/>
+        <v>https://www.veza.ru/produktsiya/klapany-i-setevye-elementy/vozdushnye-klapany/pryamougolnye-vozdushnye-klapany/germik-p-r-c-pryamougolnyy</v>
       </c>
       <c r="O123" t="str">
         <f>IF(Компоненты!O123&lt;&gt;"",Компоненты!O123,"")</f>
-        <v/>
+        <v>Все</v>
       </c>
       <c r="P123" t="str">
         <f>IF(Компоненты!P123&lt;&gt;"",Компоненты!P123,"")</f>
-        <v/>
+        <v>2025.02.18</v>
       </c>
       <c r="Q123" t="str">
         <f>IF(Компоненты!Q123&lt;&gt;"",Компоненты!Q123,"")</f>
@@ -19611,49 +20272,53 @@
       </c>
     </row>
     <row r="124" spans="2:21">
-      <c r="B124" t="str">
+      <c r="B124">
         <f>IF(Компоненты!B124&lt;&gt;"",Компоненты!B124,"")</f>
-        <v/>
+        <v>121</v>
       </c>
       <c r="C124" t="str">
         <f>IF(Компоненты!C124&lt;&gt;"",Компоненты!C124,"")</f>
-        <v/>
-      </c>
-      <c r="D124" t="str">
+        <v>Нерпа, круглый</v>
+      </c>
+      <c r="D124">
         <f>IF(Компоненты!D124&lt;&gt;"",Компоненты!D124,"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="E124" t="str">
         <f>IF(Компоненты!E124&lt;&gt;"",Компоненты!E124,"")</f>
-        <v/>
+        <v>a97f7fe17eabd99172b246a30495017c</v>
       </c>
       <c r="F124" t="str">
         <f>IF(Компоненты!F124&lt;&gt;"",Компоненты!F124,"")</f>
-        <v/>
+        <v>Арматура воздуховодов</v>
       </c>
       <c r="G124" t="str">
         <f>IF(Компоненты!G124&lt;&gt;"",Компоненты!G124,"")</f>
-        <v/>
+        <v>Клапан воздушный</v>
       </c>
       <c r="H124" t="str">
         <f>IF(Компоненты!H124&lt;&gt;"",Компоненты!H124,"")</f>
-        <v/>
+        <v>высокой плотности</v>
       </c>
       <c r="I124" t="str">
         <f>IF(Компоненты!I124&lt;&gt;"",Компоненты!I124,"")</f>
-        <v/>
+        <v>Круглый</v>
       </c>
       <c r="J124" t="str">
         <f>IF(Компоненты!J124&lt;&gt;"",Компоненты!J124,"")</f>
-        <v/>
+        <v>Веза</v>
       </c>
       <c r="K124" t="str">
         <f>IF(Компоненты!K124&lt;&gt;"",Компоненты!K124,"")</f>
-        <v/>
+        <v>Параметрическая</v>
       </c>
       <c r="L124" t="str">
         <f>IF(Компоненты!L124&lt;&gt;"",Компоненты!L124,"")</f>
-        <v/>
+        <v>3 версии компонента в одном *.repository:
+- с ручкой
+- с приводом ЭП
+- с приводом ЭПВ
+Параметризованы все габариты, количество приводов, автоматический подбор количества лопаток, артикул автоформируемый, защита от неправильных габаритов</v>
       </c>
       <c r="M124" t="str">
         <f>IF(Компоненты!M124&lt;&gt;"",Компоненты!M124,"")</f>
@@ -19661,15 +20326,15 @@
       </c>
       <c r="N124" t="str">
         <f>IF(Компоненты!N124&lt;&gt;"",Компоненты!N124,"")</f>
-        <v/>
+        <v>https://www.veza.ru/produktsiya/klapany-i-setevye-elementy/vozdushnye-klapany/kruglye-vozdushnye-klapany/nerpa-kruglyy</v>
       </c>
       <c r="O124" t="str">
         <f>IF(Компоненты!O124&lt;&gt;"",Компоненты!O124,"")</f>
-        <v/>
+        <v>Все</v>
       </c>
       <c r="P124" t="str">
         <f>IF(Компоненты!P124&lt;&gt;"",Компоненты!P124,"")</f>
-        <v/>
+        <v>2025.02.18</v>
       </c>
       <c r="Q124" t="str">
         <f>IF(Компоненты!Q124&lt;&gt;"",Компоненты!Q124,"")</f>
@@ -19693,29 +20358,29 @@
       </c>
     </row>
     <row r="125" spans="2:21">
-      <c r="B125" t="str">
+      <c r="B125">
         <f>IF(Компоненты!B125&lt;&gt;"",Компоненты!B125,"")</f>
-        <v/>
+        <v>122</v>
       </c>
       <c r="C125" t="str">
         <f>IF(Компоненты!C125&lt;&gt;"",Компоненты!C125,"")</f>
-        <v/>
-      </c>
-      <c r="D125" t="str">
+        <v>Манометр</v>
+      </c>
+      <c r="D125">
         <f>IF(Компоненты!D125&lt;&gt;"",Компоненты!D125,"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="E125" t="str">
         <f>IF(Компоненты!E125&lt;&gt;"",Компоненты!E125,"")</f>
-        <v/>
+        <v>b6e48805009c9270cffaeaac90aff34c</v>
       </c>
       <c r="F125" t="str">
         <f>IF(Компоненты!F125&lt;&gt;"",Компоненты!F125,"")</f>
-        <v/>
+        <v>Контрольно-измерительные приборы</v>
       </c>
       <c r="G125" t="str">
         <f>IF(Компоненты!G125&lt;&gt;"",Компоненты!G125,"")</f>
-        <v/>
+        <v>Термометры и манометры</v>
       </c>
       <c r="H125" t="str">
         <f>IF(Компоненты!H125&lt;&gt;"",Компоненты!H125,"")</f>
@@ -19723,19 +20388,19 @@
       </c>
       <c r="I125" t="str">
         <f>IF(Компоненты!I125&lt;&gt;"",Компоненты!I125,"")</f>
-        <v/>
+        <v>Не применимо</v>
       </c>
       <c r="J125" t="str">
         <f>IF(Компоненты!J125&lt;&gt;"",Компоненты!J125,"")</f>
-        <v/>
+        <v>Базовое оборудование</v>
       </c>
       <c r="K125" t="str">
         <f>IF(Компоненты!K125&lt;&gt;"",Компоненты!K125,"")</f>
-        <v/>
+        <v>Параметрическая</v>
       </c>
       <c r="L125" t="str">
         <f>IF(Компоненты!L125&lt;&gt;"",Компоненты!L125,"")</f>
-        <v/>
+        <v>Термометр с гильзой и бобышкой</v>
       </c>
       <c r="M125" t="str">
         <f>IF(Компоненты!M125&lt;&gt;"",Компоненты!M125,"")</f>
@@ -19747,11 +20412,11 @@
       </c>
       <c r="O125" t="str">
         <f>IF(Компоненты!O125&lt;&gt;"",Компоненты!O125,"")</f>
-        <v/>
+        <v>D63, D100</v>
       </c>
       <c r="P125" t="str">
         <f>IF(Компоненты!P125&lt;&gt;"",Компоненты!P125,"")</f>
-        <v/>
+        <v>2025.02.18</v>
       </c>
       <c r="Q125" t="str">
         <f>IF(Компоненты!Q125&lt;&gt;"",Компоненты!Q125,"")</f>
@@ -19775,29 +20440,29 @@
       </c>
     </row>
     <row r="126" spans="2:21">
-      <c r="B126" t="str">
+      <c r="B126">
         <f>IF(Компоненты!B126&lt;&gt;"",Компоненты!B126,"")</f>
-        <v/>
+        <v>123</v>
       </c>
       <c r="C126" t="str">
         <f>IF(Компоненты!C126&lt;&gt;"",Компоненты!C126,"")</f>
-        <v/>
-      </c>
-      <c r="D126" t="str">
+        <v>Термометр</v>
+      </c>
+      <c r="D126">
         <f>IF(Компоненты!D126&lt;&gt;"",Компоненты!D126,"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="E126" t="str">
         <f>IF(Компоненты!E126&lt;&gt;"",Компоненты!E126,"")</f>
-        <v/>
+        <v>319f3017a48f460bc38ab3a271a80a09</v>
       </c>
       <c r="F126" t="str">
         <f>IF(Компоненты!F126&lt;&gt;"",Компоненты!F126,"")</f>
-        <v/>
+        <v>Контрольно-измерительные приборы</v>
       </c>
       <c r="G126" t="str">
         <f>IF(Компоненты!G126&lt;&gt;"",Компоненты!G126,"")</f>
-        <v/>
+        <v>Термометры и манометры</v>
       </c>
       <c r="H126" t="str">
         <f>IF(Компоненты!H126&lt;&gt;"",Компоненты!H126,"")</f>
@@ -19805,19 +20470,19 @@
       </c>
       <c r="I126" t="str">
         <f>IF(Компоненты!I126&lt;&gt;"",Компоненты!I126,"")</f>
-        <v/>
+        <v>Не применимо</v>
       </c>
       <c r="J126" t="str">
         <f>IF(Компоненты!J126&lt;&gt;"",Компоненты!J126,"")</f>
-        <v/>
+        <v>Базовое оборудование</v>
       </c>
       <c r="K126" t="str">
         <f>IF(Компоненты!K126&lt;&gt;"",Компоненты!K126,"")</f>
-        <v/>
+        <v>Параметрическая</v>
       </c>
       <c r="L126" t="str">
         <f>IF(Компоненты!L126&lt;&gt;"",Компоненты!L126,"")</f>
-        <v/>
+        <v>Манометр с трехходовым краном и бобышкой</v>
       </c>
       <c r="M126" t="str">
         <f>IF(Компоненты!M126&lt;&gt;"",Компоненты!M126,"")</f>
@@ -19829,11 +20494,11 @@
       </c>
       <c r="O126" t="str">
         <f>IF(Компоненты!O126&lt;&gt;"",Компоненты!O126,"")</f>
-        <v/>
+        <v>D40, D150</v>
       </c>
       <c r="P126" t="str">
         <f>IF(Компоненты!P126&lt;&gt;"",Компоненты!P126,"")</f>
-        <v/>
+        <v>2025.02.18</v>
       </c>
       <c r="Q126" t="str">
         <f>IF(Компоненты!Q126&lt;&gt;"",Компоненты!Q126,"")</f>
@@ -25270,657 +25935,657 @@
     </row>
     <row r="193" spans="2:21">
       <c r="B193" t="str">
-        <f>IF(Компоненты!B193&lt;&gt;"",Компоненты!B193,"")</f>
+        <f>IF(Компоненты!B202&lt;&gt;"",Компоненты!B202,"")</f>
         <v/>
       </c>
       <c r="C193" t="str">
-        <f>IF(Компоненты!C193&lt;&gt;"",Компоненты!C193,"")</f>
+        <f>IF(Компоненты!C202&lt;&gt;"",Компоненты!C202,"")</f>
         <v/>
       </c>
       <c r="D193" t="str">
-        <f>IF(Компоненты!D193&lt;&gt;"",Компоненты!D193,"")</f>
+        <f>IF(Компоненты!D202&lt;&gt;"",Компоненты!D202,"")</f>
         <v/>
       </c>
       <c r="E193" t="str">
-        <f>IF(Компоненты!E193&lt;&gt;"",Компоненты!E193,"")</f>
+        <f>IF(Компоненты!E202&lt;&gt;"",Компоненты!E202,"")</f>
         <v/>
       </c>
       <c r="F193" t="str">
-        <f>IF(Компоненты!F193&lt;&gt;"",Компоненты!F193,"")</f>
+        <f>IF(Компоненты!F202&lt;&gt;"",Компоненты!F202,"")</f>
         <v/>
       </c>
       <c r="G193" t="str">
-        <f>IF(Компоненты!G193&lt;&gt;"",Компоненты!G193,"")</f>
+        <f>IF(Компоненты!G202&lt;&gt;"",Компоненты!G202,"")</f>
         <v/>
       </c>
       <c r="H193" t="str">
-        <f>IF(Компоненты!H193&lt;&gt;"",Компоненты!H193,"")</f>
+        <f>IF(Компоненты!H202&lt;&gt;"",Компоненты!H202,"")</f>
         <v/>
       </c>
       <c r="I193" t="str">
-        <f>IF(Компоненты!I193&lt;&gt;"",Компоненты!I193,"")</f>
+        <f>IF(Компоненты!I202&lt;&gt;"",Компоненты!I202,"")</f>
         <v/>
       </c>
       <c r="J193" t="str">
-        <f>IF(Компоненты!J193&lt;&gt;"",Компоненты!J193,"")</f>
+        <f>IF(Компоненты!J202&lt;&gt;"",Компоненты!J202,"")</f>
         <v/>
       </c>
       <c r="K193" t="str">
-        <f>IF(Компоненты!K193&lt;&gt;"",Компоненты!K193,"")</f>
+        <f>IF(Компоненты!K202&lt;&gt;"",Компоненты!K202,"")</f>
         <v/>
       </c>
       <c r="L193" t="str">
-        <f>IF(Компоненты!L193&lt;&gt;"",Компоненты!L193,"")</f>
+        <f>IF(Компоненты!L202&lt;&gt;"",Компоненты!L202,"")</f>
         <v/>
       </c>
       <c r="M193" t="str">
-        <f>IF(Компоненты!M193&lt;&gt;"",Компоненты!M193,"")</f>
+        <f>IF(Компоненты!M202&lt;&gt;"",Компоненты!M202,"")</f>
         <v/>
       </c>
       <c r="N193" t="str">
-        <f>IF(Компоненты!N193&lt;&gt;"",Компоненты!N193,"")</f>
+        <f>IF(Компоненты!N202&lt;&gt;"",Компоненты!N202,"")</f>
         <v/>
       </c>
       <c r="O193" t="str">
-        <f>IF(Компоненты!O193&lt;&gt;"",Компоненты!O193,"")</f>
+        <f>IF(Компоненты!O202&lt;&gt;"",Компоненты!O202,"")</f>
         <v/>
       </c>
       <c r="P193" t="str">
-        <f>IF(Компоненты!P193&lt;&gt;"",Компоненты!P193,"")</f>
+        <f>IF(Компоненты!P202&lt;&gt;"",Компоненты!P202,"")</f>
         <v/>
       </c>
       <c r="Q193" t="str">
-        <f>IF(Компоненты!Q193&lt;&gt;"",Компоненты!Q193,"")</f>
+        <f>IF(Компоненты!Q202&lt;&gt;"",Компоненты!Q202,"")</f>
         <v/>
       </c>
       <c r="R193" t="str">
-        <f>IF(Компоненты!R193&lt;&gt;"",Компоненты!R193,"")</f>
+        <f>IF(Компоненты!R202&lt;&gt;"",Компоненты!R202,"")</f>
         <v/>
       </c>
       <c r="S193" t="str">
-        <f>IF(Компоненты!S193&lt;&gt;"",Компоненты!S193,"")</f>
+        <f>IF(Компоненты!S202&lt;&gt;"",Компоненты!S202,"")</f>
         <v/>
       </c>
       <c r="T193" t="str">
-        <f>IF(Компоненты!T193&lt;&gt;"",Компоненты!T193,"")</f>
+        <f>IF(Компоненты!T202&lt;&gt;"",Компоненты!T202,"")</f>
         <v/>
       </c>
       <c r="U193" t="str">
-        <f>IF(Компоненты!U193&lt;&gt;"",Компоненты!U193,"")</f>
+        <f>IF(Компоненты!U202&lt;&gt;"",Компоненты!U202,"")</f>
         <v/>
       </c>
     </row>
     <row r="194" spans="2:21">
       <c r="B194" t="str">
-        <f>IF(Компоненты!B194&lt;&gt;"",Компоненты!B194,"")</f>
+        <f>IF(Компоненты!B203&lt;&gt;"",Компоненты!B203,"")</f>
         <v/>
       </c>
       <c r="C194" t="str">
-        <f>IF(Компоненты!C194&lt;&gt;"",Компоненты!C194,"")</f>
+        <f>IF(Компоненты!C203&lt;&gt;"",Компоненты!C203,"")</f>
         <v/>
       </c>
       <c r="D194" t="str">
-        <f>IF(Компоненты!D194&lt;&gt;"",Компоненты!D194,"")</f>
+        <f>IF(Компоненты!D203&lt;&gt;"",Компоненты!D203,"")</f>
         <v/>
       </c>
       <c r="E194" t="str">
-        <f>IF(Компоненты!E194&lt;&gt;"",Компоненты!E194,"")</f>
+        <f>IF(Компоненты!E203&lt;&gt;"",Компоненты!E203,"")</f>
         <v/>
       </c>
       <c r="F194" t="str">
-        <f>IF(Компоненты!F194&lt;&gt;"",Компоненты!F194,"")</f>
+        <f>IF(Компоненты!F203&lt;&gt;"",Компоненты!F203,"")</f>
         <v/>
       </c>
       <c r="G194" t="str">
-        <f>IF(Компоненты!G194&lt;&gt;"",Компоненты!G194,"")</f>
+        <f>IF(Компоненты!G203&lt;&gt;"",Компоненты!G203,"")</f>
         <v/>
       </c>
       <c r="H194" t="str">
-        <f>IF(Компоненты!H194&lt;&gt;"",Компоненты!H194,"")</f>
+        <f>IF(Компоненты!H203&lt;&gt;"",Компоненты!H203,"")</f>
         <v/>
       </c>
       <c r="I194" t="str">
-        <f>IF(Компоненты!I194&lt;&gt;"",Компоненты!I194,"")</f>
+        <f>IF(Компоненты!I203&lt;&gt;"",Компоненты!I203,"")</f>
         <v/>
       </c>
       <c r="J194" t="str">
-        <f>IF(Компоненты!J194&lt;&gt;"",Компоненты!J194,"")</f>
+        <f>IF(Компоненты!J203&lt;&gt;"",Компоненты!J203,"")</f>
         <v/>
       </c>
       <c r="K194" t="str">
-        <f>IF(Компоненты!K194&lt;&gt;"",Компоненты!K194,"")</f>
+        <f>IF(Компоненты!K203&lt;&gt;"",Компоненты!K203,"")</f>
         <v/>
       </c>
       <c r="L194" t="str">
-        <f>IF(Компоненты!L194&lt;&gt;"",Компоненты!L194,"")</f>
+        <f>IF(Компоненты!L203&lt;&gt;"",Компоненты!L203,"")</f>
         <v/>
       </c>
       <c r="M194" t="str">
-        <f>IF(Компоненты!M194&lt;&gt;"",Компоненты!M194,"")</f>
+        <f>IF(Компоненты!M203&lt;&gt;"",Компоненты!M203,"")</f>
         <v/>
       </c>
       <c r="N194" t="str">
-        <f>IF(Компоненты!N194&lt;&gt;"",Компоненты!N194,"")</f>
+        <f>IF(Компоненты!N203&lt;&gt;"",Компоненты!N203,"")</f>
         <v/>
       </c>
       <c r="O194" t="str">
-        <f>IF(Компоненты!O194&lt;&gt;"",Компоненты!O194,"")</f>
+        <f>IF(Компоненты!O203&lt;&gt;"",Компоненты!O203,"")</f>
         <v/>
       </c>
       <c r="P194" t="str">
-        <f>IF(Компоненты!P194&lt;&gt;"",Компоненты!P194,"")</f>
+        <f>IF(Компоненты!P203&lt;&gt;"",Компоненты!P203,"")</f>
         <v/>
       </c>
       <c r="Q194" t="str">
-        <f>IF(Компоненты!Q194&lt;&gt;"",Компоненты!Q194,"")</f>
+        <f>IF(Компоненты!Q203&lt;&gt;"",Компоненты!Q203,"")</f>
         <v/>
       </c>
       <c r="R194" t="str">
-        <f>IF(Компоненты!R194&lt;&gt;"",Компоненты!R194,"")</f>
+        <f>IF(Компоненты!R203&lt;&gt;"",Компоненты!R203,"")</f>
         <v/>
       </c>
       <c r="S194" t="str">
-        <f>IF(Компоненты!S194&lt;&gt;"",Компоненты!S194,"")</f>
+        <f>IF(Компоненты!S203&lt;&gt;"",Компоненты!S203,"")</f>
         <v/>
       </c>
       <c r="T194" t="str">
-        <f>IF(Компоненты!T194&lt;&gt;"",Компоненты!T194,"")</f>
+        <f>IF(Компоненты!T203&lt;&gt;"",Компоненты!T203,"")</f>
         <v/>
       </c>
       <c r="U194" t="str">
-        <f>IF(Компоненты!U194&lt;&gt;"",Компоненты!U194,"")</f>
+        <f>IF(Компоненты!U203&lt;&gt;"",Компоненты!U203,"")</f>
         <v/>
       </c>
     </row>
     <row r="195" spans="2:21">
       <c r="B195" t="str">
-        <f>IF(Компоненты!B195&lt;&gt;"",Компоненты!B195,"")</f>
+        <f>IF(Компоненты!B204&lt;&gt;"",Компоненты!B204,"")</f>
         <v/>
       </c>
       <c r="C195" t="str">
-        <f>IF(Компоненты!C195&lt;&gt;"",Компоненты!C195,"")</f>
+        <f>IF(Компоненты!C204&lt;&gt;"",Компоненты!C204,"")</f>
         <v/>
       </c>
       <c r="D195" t="str">
-        <f>IF(Компоненты!D195&lt;&gt;"",Компоненты!D195,"")</f>
+        <f>IF(Компоненты!D204&lt;&gt;"",Компоненты!D204,"")</f>
         <v/>
       </c>
       <c r="E195" t="str">
-        <f>IF(Компоненты!E195&lt;&gt;"",Компоненты!E195,"")</f>
+        <f>IF(Компоненты!E204&lt;&gt;"",Компоненты!E204,"")</f>
         <v/>
       </c>
       <c r="F195" t="str">
-        <f>IF(Компоненты!F195&lt;&gt;"",Компоненты!F195,"")</f>
+        <f>IF(Компоненты!F204&lt;&gt;"",Компоненты!F204,"")</f>
         <v/>
       </c>
       <c r="G195" t="str">
-        <f>IF(Компоненты!G195&lt;&gt;"",Компоненты!G195,"")</f>
+        <f>IF(Компоненты!G204&lt;&gt;"",Компоненты!G204,"")</f>
         <v/>
       </c>
       <c r="H195" t="str">
-        <f>IF(Компоненты!H195&lt;&gt;"",Компоненты!H195,"")</f>
+        <f>IF(Компоненты!H204&lt;&gt;"",Компоненты!H204,"")</f>
         <v/>
       </c>
       <c r="I195" t="str">
-        <f>IF(Компоненты!I195&lt;&gt;"",Компоненты!I195,"")</f>
+        <f>IF(Компоненты!I204&lt;&gt;"",Компоненты!I204,"")</f>
         <v/>
       </c>
       <c r="J195" t="str">
-        <f>IF(Компоненты!J195&lt;&gt;"",Компоненты!J195,"")</f>
+        <f>IF(Компоненты!J204&lt;&gt;"",Компоненты!J204,"")</f>
         <v/>
       </c>
       <c r="K195" t="str">
-        <f>IF(Компоненты!K195&lt;&gt;"",Компоненты!K195,"")</f>
+        <f>IF(Компоненты!K204&lt;&gt;"",Компоненты!K204,"")</f>
         <v/>
       </c>
       <c r="L195" t="str">
-        <f>IF(Компоненты!L195&lt;&gt;"",Компоненты!L195,"")</f>
+        <f>IF(Компоненты!L204&lt;&gt;"",Компоненты!L204,"")</f>
         <v/>
       </c>
       <c r="M195" t="str">
-        <f>IF(Компоненты!M195&lt;&gt;"",Компоненты!M195,"")</f>
+        <f>IF(Компоненты!M204&lt;&gt;"",Компоненты!M204,"")</f>
         <v/>
       </c>
       <c r="N195" t="str">
-        <f>IF(Компоненты!N195&lt;&gt;"",Компоненты!N195,"")</f>
+        <f>IF(Компоненты!N204&lt;&gt;"",Компоненты!N204,"")</f>
         <v/>
       </c>
       <c r="O195" t="str">
-        <f>IF(Компоненты!O195&lt;&gt;"",Компоненты!O195,"")</f>
+        <f>IF(Компоненты!O204&lt;&gt;"",Компоненты!O204,"")</f>
         <v/>
       </c>
       <c r="P195" t="str">
-        <f>IF(Компоненты!P195&lt;&gt;"",Компоненты!P195,"")</f>
+        <f>IF(Компоненты!P204&lt;&gt;"",Компоненты!P204,"")</f>
         <v/>
       </c>
       <c r="Q195" t="str">
-        <f>IF(Компоненты!Q195&lt;&gt;"",Компоненты!Q195,"")</f>
+        <f>IF(Компоненты!Q204&lt;&gt;"",Компоненты!Q204,"")</f>
         <v/>
       </c>
       <c r="R195" t="str">
-        <f>IF(Компоненты!R195&lt;&gt;"",Компоненты!R195,"")</f>
+        <f>IF(Компоненты!R204&lt;&gt;"",Компоненты!R204,"")</f>
         <v/>
       </c>
       <c r="S195" t="str">
-        <f>IF(Компоненты!S195&lt;&gt;"",Компоненты!S195,"")</f>
+        <f>IF(Компоненты!S204&lt;&gt;"",Компоненты!S204,"")</f>
         <v/>
       </c>
       <c r="T195" t="str">
-        <f>IF(Компоненты!T195&lt;&gt;"",Компоненты!T195,"")</f>
+        <f>IF(Компоненты!T204&lt;&gt;"",Компоненты!T204,"")</f>
         <v/>
       </c>
       <c r="U195" t="str">
-        <f>IF(Компоненты!U195&lt;&gt;"",Компоненты!U195,"")</f>
+        <f>IF(Компоненты!U204&lt;&gt;"",Компоненты!U204,"")</f>
         <v/>
       </c>
     </row>
     <row r="196" spans="2:21">
       <c r="B196" t="str">
-        <f>IF(Компоненты!B196&lt;&gt;"",Компоненты!B196,"")</f>
+        <f>IF(Компоненты!B205&lt;&gt;"",Компоненты!B205,"")</f>
         <v/>
       </c>
       <c r="C196" t="str">
-        <f>IF(Компоненты!C196&lt;&gt;"",Компоненты!C196,"")</f>
+        <f>IF(Компоненты!C205&lt;&gt;"",Компоненты!C205,"")</f>
         <v/>
       </c>
       <c r="D196" t="str">
-        <f>IF(Компоненты!D196&lt;&gt;"",Компоненты!D196,"")</f>
+        <f>IF(Компоненты!D205&lt;&gt;"",Компоненты!D205,"")</f>
         <v/>
       </c>
       <c r="E196" t="str">
-        <f>IF(Компоненты!E196&lt;&gt;"",Компоненты!E196,"")</f>
+        <f>IF(Компоненты!E205&lt;&gt;"",Компоненты!E205,"")</f>
         <v/>
       </c>
       <c r="F196" t="str">
-        <f>IF(Компоненты!F196&lt;&gt;"",Компоненты!F196,"")</f>
+        <f>IF(Компоненты!F205&lt;&gt;"",Компоненты!F205,"")</f>
         <v/>
       </c>
       <c r="G196" t="str">
-        <f>IF(Компоненты!G196&lt;&gt;"",Компоненты!G196,"")</f>
+        <f>IF(Компоненты!G205&lt;&gt;"",Компоненты!G205,"")</f>
         <v/>
       </c>
       <c r="H196" t="str">
-        <f>IF(Компоненты!H196&lt;&gt;"",Компоненты!H196,"")</f>
+        <f>IF(Компоненты!H205&lt;&gt;"",Компоненты!H205,"")</f>
         <v/>
       </c>
       <c r="I196" t="str">
-        <f>IF(Компоненты!I196&lt;&gt;"",Компоненты!I196,"")</f>
+        <f>IF(Компоненты!I205&lt;&gt;"",Компоненты!I205,"")</f>
         <v/>
       </c>
       <c r="J196" t="str">
-        <f>IF(Компоненты!J196&lt;&gt;"",Компоненты!J196,"")</f>
+        <f>IF(Компоненты!J205&lt;&gt;"",Компоненты!J205,"")</f>
         <v/>
       </c>
       <c r="K196" t="str">
-        <f>IF(Компоненты!K196&lt;&gt;"",Компоненты!K196,"")</f>
+        <f>IF(Компоненты!K205&lt;&gt;"",Компоненты!K205,"")</f>
         <v/>
       </c>
       <c r="L196" t="str">
-        <f>IF(Компоненты!L196&lt;&gt;"",Компоненты!L196,"")</f>
+        <f>IF(Компоненты!L205&lt;&gt;"",Компоненты!L205,"")</f>
         <v/>
       </c>
       <c r="M196" t="str">
-        <f>IF(Компоненты!M196&lt;&gt;"",Компоненты!M196,"")</f>
+        <f>IF(Компоненты!M205&lt;&gt;"",Компоненты!M205,"")</f>
         <v/>
       </c>
       <c r="N196" t="str">
-        <f>IF(Компоненты!N196&lt;&gt;"",Компоненты!N196,"")</f>
+        <f>IF(Компоненты!N205&lt;&gt;"",Компоненты!N205,"")</f>
         <v/>
       </c>
       <c r="O196" t="str">
-        <f>IF(Компоненты!O196&lt;&gt;"",Компоненты!O196,"")</f>
+        <f>IF(Компоненты!O205&lt;&gt;"",Компоненты!O205,"")</f>
         <v/>
       </c>
       <c r="P196" t="str">
-        <f>IF(Компоненты!P196&lt;&gt;"",Компоненты!P196,"")</f>
+        <f>IF(Компоненты!P205&lt;&gt;"",Компоненты!P205,"")</f>
         <v/>
       </c>
       <c r="Q196" t="str">
-        <f>IF(Компоненты!Q196&lt;&gt;"",Компоненты!Q196,"")</f>
+        <f>IF(Компоненты!Q205&lt;&gt;"",Компоненты!Q205,"")</f>
         <v/>
       </c>
       <c r="R196" t="str">
-        <f>IF(Компоненты!R196&lt;&gt;"",Компоненты!R196,"")</f>
+        <f>IF(Компоненты!R205&lt;&gt;"",Компоненты!R205,"")</f>
         <v/>
       </c>
       <c r="S196" t="str">
-        <f>IF(Компоненты!S196&lt;&gt;"",Компоненты!S196,"")</f>
+        <f>IF(Компоненты!S205&lt;&gt;"",Компоненты!S205,"")</f>
         <v/>
       </c>
       <c r="T196" t="str">
-        <f>IF(Компоненты!T196&lt;&gt;"",Компоненты!T196,"")</f>
+        <f>IF(Компоненты!T205&lt;&gt;"",Компоненты!T205,"")</f>
         <v/>
       </c>
       <c r="U196" t="str">
-        <f>IF(Компоненты!U196&lt;&gt;"",Компоненты!U196,"")</f>
+        <f>IF(Компоненты!U205&lt;&gt;"",Компоненты!U205,"")</f>
         <v/>
       </c>
     </row>
     <row r="197" spans="2:21">
       <c r="B197" t="str">
-        <f>IF(Компоненты!B197&lt;&gt;"",Компоненты!B197,"")</f>
+        <f>IF(Компоненты!B206&lt;&gt;"",Компоненты!B206,"")</f>
         <v/>
       </c>
       <c r="C197" t="str">
-        <f>IF(Компоненты!C197&lt;&gt;"",Компоненты!C197,"")</f>
+        <f>IF(Компоненты!C206&lt;&gt;"",Компоненты!C206,"")</f>
         <v/>
       </c>
       <c r="D197" t="str">
-        <f>IF(Компоненты!D197&lt;&gt;"",Компоненты!D197,"")</f>
+        <f>IF(Компоненты!D206&lt;&gt;"",Компоненты!D206,"")</f>
         <v/>
       </c>
       <c r="E197" t="str">
-        <f>IF(Компоненты!E197&lt;&gt;"",Компоненты!E197,"")</f>
+        <f>IF(Компоненты!E206&lt;&gt;"",Компоненты!E206,"")</f>
         <v/>
       </c>
       <c r="F197" t="str">
-        <f>IF(Компоненты!F197&lt;&gt;"",Компоненты!F197,"")</f>
+        <f>IF(Компоненты!F206&lt;&gt;"",Компоненты!F206,"")</f>
         <v/>
       </c>
       <c r="G197" t="str">
-        <f>IF(Компоненты!G197&lt;&gt;"",Компоненты!G197,"")</f>
+        <f>IF(Компоненты!G206&lt;&gt;"",Компоненты!G206,"")</f>
         <v/>
       </c>
       <c r="H197" t="str">
-        <f>IF(Компоненты!H197&lt;&gt;"",Компоненты!H197,"")</f>
+        <f>IF(Компоненты!H206&lt;&gt;"",Компоненты!H206,"")</f>
         <v/>
       </c>
       <c r="I197" t="str">
-        <f>IF(Компоненты!I197&lt;&gt;"",Компоненты!I197,"")</f>
+        <f>IF(Компоненты!I206&lt;&gt;"",Компоненты!I206,"")</f>
         <v/>
       </c>
       <c r="J197" t="str">
-        <f>IF(Компоненты!J197&lt;&gt;"",Компоненты!J197,"")</f>
+        <f>IF(Компоненты!J206&lt;&gt;"",Компоненты!J206,"")</f>
         <v/>
       </c>
       <c r="K197" t="str">
-        <f>IF(Компоненты!K197&lt;&gt;"",Компоненты!K197,"")</f>
+        <f>IF(Компоненты!K206&lt;&gt;"",Компоненты!K206,"")</f>
         <v/>
       </c>
       <c r="L197" t="str">
-        <f>IF(Компоненты!L197&lt;&gt;"",Компоненты!L197,"")</f>
+        <f>IF(Компоненты!L206&lt;&gt;"",Компоненты!L206,"")</f>
         <v/>
       </c>
       <c r="M197" t="str">
-        <f>IF(Компоненты!M197&lt;&gt;"",Компоненты!M197,"")</f>
+        <f>IF(Компоненты!M206&lt;&gt;"",Компоненты!M206,"")</f>
         <v/>
       </c>
       <c r="N197" t="str">
-        <f>IF(Компоненты!N197&lt;&gt;"",Компоненты!N197,"")</f>
+        <f>IF(Компоненты!N206&lt;&gt;"",Компоненты!N206,"")</f>
         <v/>
       </c>
       <c r="O197" t="str">
-        <f>IF(Компоненты!O197&lt;&gt;"",Компоненты!O197,"")</f>
+        <f>IF(Компоненты!O206&lt;&gt;"",Компоненты!O206,"")</f>
         <v/>
       </c>
       <c r="P197" t="str">
-        <f>IF(Компоненты!P197&lt;&gt;"",Компоненты!P197,"")</f>
+        <f>IF(Компоненты!P206&lt;&gt;"",Компоненты!P206,"")</f>
         <v/>
       </c>
       <c r="Q197" t="str">
-        <f>IF(Компоненты!Q197&lt;&gt;"",Компоненты!Q197,"")</f>
+        <f>IF(Компоненты!Q206&lt;&gt;"",Компоненты!Q206,"")</f>
         <v/>
       </c>
       <c r="R197" t="str">
-        <f>IF(Компоненты!R197&lt;&gt;"",Компоненты!R197,"")</f>
+        <f>IF(Компоненты!R206&lt;&gt;"",Компоненты!R206,"")</f>
         <v/>
       </c>
       <c r="S197" t="str">
-        <f>IF(Компоненты!S197&lt;&gt;"",Компоненты!S197,"")</f>
+        <f>IF(Компоненты!S206&lt;&gt;"",Компоненты!S206,"")</f>
         <v/>
       </c>
       <c r="T197" t="str">
-        <f>IF(Компоненты!T197&lt;&gt;"",Компоненты!T197,"")</f>
+        <f>IF(Компоненты!T206&lt;&gt;"",Компоненты!T206,"")</f>
         <v/>
       </c>
       <c r="U197" t="str">
-        <f>IF(Компоненты!U197&lt;&gt;"",Компоненты!U197,"")</f>
+        <f>IF(Компоненты!U206&lt;&gt;"",Компоненты!U206,"")</f>
         <v/>
       </c>
     </row>
     <row r="198" spans="2:21">
       <c r="B198" t="str">
-        <f>IF(Компоненты!B198&lt;&gt;"",Компоненты!B198,"")</f>
+        <f>IF(Компоненты!B207&lt;&gt;"",Компоненты!B207,"")</f>
         <v/>
       </c>
       <c r="C198" t="str">
-        <f>IF(Компоненты!C198&lt;&gt;"",Компоненты!C198,"")</f>
+        <f>IF(Компоненты!C207&lt;&gt;"",Компоненты!C207,"")</f>
         <v/>
       </c>
       <c r="D198" t="str">
-        <f>IF(Компоненты!D198&lt;&gt;"",Компоненты!D198,"")</f>
+        <f>IF(Компоненты!D207&lt;&gt;"",Компоненты!D207,"")</f>
         <v/>
       </c>
       <c r="E198" t="str">
-        <f>IF(Компоненты!E198&lt;&gt;"",Компоненты!E198,"")</f>
+        <f>IF(Компоненты!E207&lt;&gt;"",Компоненты!E207,"")</f>
         <v/>
       </c>
       <c r="F198" t="str">
-        <f>IF(Компоненты!F198&lt;&gt;"",Компоненты!F198,"")</f>
+        <f>IF(Компоненты!F207&lt;&gt;"",Компоненты!F207,"")</f>
         <v/>
       </c>
       <c r="G198" t="str">
-        <f>IF(Компоненты!G198&lt;&gt;"",Компоненты!G198,"")</f>
+        <f>IF(Компоненты!G207&lt;&gt;"",Компоненты!G207,"")</f>
         <v/>
       </c>
       <c r="H198" t="str">
-        <f>IF(Компоненты!H198&lt;&gt;"",Компоненты!H198,"")</f>
+        <f>IF(Компоненты!H207&lt;&gt;"",Компоненты!H207,"")</f>
         <v/>
       </c>
       <c r="I198" t="str">
-        <f>IF(Компоненты!I198&lt;&gt;"",Компоненты!I198,"")</f>
+        <f>IF(Компоненты!I207&lt;&gt;"",Компоненты!I207,"")</f>
         <v/>
       </c>
       <c r="J198" t="str">
-        <f>IF(Компоненты!J198&lt;&gt;"",Компоненты!J198,"")</f>
+        <f>IF(Компоненты!J207&lt;&gt;"",Компоненты!J207,"")</f>
         <v/>
       </c>
       <c r="K198" t="str">
-        <f>IF(Компоненты!K198&lt;&gt;"",Компоненты!K198,"")</f>
+        <f>IF(Компоненты!K207&lt;&gt;"",Компоненты!K207,"")</f>
         <v/>
       </c>
       <c r="L198" t="str">
-        <f>IF(Компоненты!L198&lt;&gt;"",Компоненты!L198,"")</f>
+        <f>IF(Компоненты!L207&lt;&gt;"",Компоненты!L207,"")</f>
         <v/>
       </c>
       <c r="M198" t="str">
-        <f>IF(Компоненты!M198&lt;&gt;"",Компоненты!M198,"")</f>
+        <f>IF(Компоненты!M207&lt;&gt;"",Компоненты!M207,"")</f>
         <v/>
       </c>
       <c r="N198" t="str">
-        <f>IF(Компоненты!N198&lt;&gt;"",Компоненты!N198,"")</f>
+        <f>IF(Компоненты!N207&lt;&gt;"",Компоненты!N207,"")</f>
         <v/>
       </c>
       <c r="O198" t="str">
-        <f>IF(Компоненты!O198&lt;&gt;"",Компоненты!O198,"")</f>
+        <f>IF(Компоненты!O207&lt;&gt;"",Компоненты!O207,"")</f>
         <v/>
       </c>
       <c r="P198" t="str">
-        <f>IF(Компоненты!P198&lt;&gt;"",Компоненты!P198,"")</f>
+        <f>IF(Компоненты!P207&lt;&gt;"",Компоненты!P207,"")</f>
         <v/>
       </c>
       <c r="Q198" t="str">
-        <f>IF(Компоненты!Q198&lt;&gt;"",Компоненты!Q198,"")</f>
+        <f>IF(Компоненты!Q207&lt;&gt;"",Компоненты!Q207,"")</f>
         <v/>
       </c>
       <c r="R198" t="str">
-        <f>IF(Компоненты!R198&lt;&gt;"",Компоненты!R198,"")</f>
+        <f>IF(Компоненты!R207&lt;&gt;"",Компоненты!R207,"")</f>
         <v/>
       </c>
       <c r="S198" t="str">
-        <f>IF(Компоненты!S198&lt;&gt;"",Компоненты!S198,"")</f>
+        <f>IF(Компоненты!S207&lt;&gt;"",Компоненты!S207,"")</f>
         <v/>
       </c>
       <c r="T198" t="str">
-        <f>IF(Компоненты!T198&lt;&gt;"",Компоненты!T198,"")</f>
+        <f>IF(Компоненты!T207&lt;&gt;"",Компоненты!T207,"")</f>
         <v/>
       </c>
       <c r="U198" t="str">
-        <f>IF(Компоненты!U198&lt;&gt;"",Компоненты!U198,"")</f>
+        <f>IF(Компоненты!U207&lt;&gt;"",Компоненты!U207,"")</f>
         <v/>
       </c>
     </row>
     <row r="199" spans="2:21">
       <c r="B199" t="str">
-        <f>IF(Компоненты!B199&lt;&gt;"",Компоненты!B199,"")</f>
+        <f>IF(Компоненты!B208&lt;&gt;"",Компоненты!B208,"")</f>
         <v/>
       </c>
       <c r="C199" t="str">
-        <f>IF(Компоненты!C199&lt;&gt;"",Компоненты!C199,"")</f>
+        <f>IF(Компоненты!C208&lt;&gt;"",Компоненты!C208,"")</f>
         <v/>
       </c>
       <c r="D199" t="str">
-        <f>IF(Компоненты!D199&lt;&gt;"",Компоненты!D199,"")</f>
+        <f>IF(Компоненты!D208&lt;&gt;"",Компоненты!D208,"")</f>
         <v/>
       </c>
       <c r="E199" t="str">
-        <f>IF(Компоненты!E199&lt;&gt;"",Компоненты!E199,"")</f>
+        <f>IF(Компоненты!E208&lt;&gt;"",Компоненты!E208,"")</f>
         <v/>
       </c>
       <c r="F199" t="str">
-        <f>IF(Компоненты!F199&lt;&gt;"",Компоненты!F199,"")</f>
+        <f>IF(Компоненты!F208&lt;&gt;"",Компоненты!F208,"")</f>
         <v/>
       </c>
       <c r="G199" t="str">
-        <f>IF(Компоненты!G199&lt;&gt;"",Компоненты!G199,"")</f>
+        <f>IF(Компоненты!G208&lt;&gt;"",Компоненты!G208,"")</f>
         <v/>
       </c>
       <c r="H199" t="str">
-        <f>IF(Компоненты!H199&lt;&gt;"",Компоненты!H199,"")</f>
+        <f>IF(Компоненты!H208&lt;&gt;"",Компоненты!H208,"")</f>
         <v/>
       </c>
       <c r="I199" t="str">
-        <f>IF(Компоненты!I199&lt;&gt;"",Компоненты!I199,"")</f>
+        <f>IF(Компоненты!I208&lt;&gt;"",Компоненты!I208,"")</f>
         <v/>
       </c>
       <c r="J199" t="str">
-        <f>IF(Компоненты!J199&lt;&gt;"",Компоненты!J199,"")</f>
+        <f>IF(Компоненты!J208&lt;&gt;"",Компоненты!J208,"")</f>
         <v/>
       </c>
       <c r="K199" t="str">
-        <f>IF(Компоненты!K199&lt;&gt;"",Компоненты!K199,"")</f>
+        <f>IF(Компоненты!K208&lt;&gt;"",Компоненты!K208,"")</f>
         <v/>
       </c>
       <c r="L199" t="str">
-        <f>IF(Компоненты!L199&lt;&gt;"",Компоненты!L199,"")</f>
+        <f>IF(Компоненты!L208&lt;&gt;"",Компоненты!L208,"")</f>
         <v/>
       </c>
       <c r="M199" t="str">
-        <f>IF(Компоненты!M199&lt;&gt;"",Компоненты!M199,"")</f>
+        <f>IF(Компоненты!M208&lt;&gt;"",Компоненты!M208,"")</f>
         <v/>
       </c>
       <c r="N199" t="str">
-        <f>IF(Компоненты!N199&lt;&gt;"",Компоненты!N199,"")</f>
+        <f>IF(Компоненты!N208&lt;&gt;"",Компоненты!N208,"")</f>
         <v/>
       </c>
       <c r="O199" t="str">
-        <f>IF(Компоненты!O199&lt;&gt;"",Компоненты!O199,"")</f>
+        <f>IF(Компоненты!O208&lt;&gt;"",Компоненты!O208,"")</f>
         <v/>
       </c>
       <c r="P199" t="str">
-        <f>IF(Компоненты!P199&lt;&gt;"",Компоненты!P199,"")</f>
+        <f>IF(Компоненты!P208&lt;&gt;"",Компоненты!P208,"")</f>
         <v/>
       </c>
       <c r="Q199" t="str">
-        <f>IF(Компоненты!Q199&lt;&gt;"",Компоненты!Q199,"")</f>
+        <f>IF(Компоненты!Q208&lt;&gt;"",Компоненты!Q208,"")</f>
         <v/>
       </c>
       <c r="R199" t="str">
-        <f>IF(Компоненты!R199&lt;&gt;"",Компоненты!R199,"")</f>
+        <f>IF(Компоненты!R208&lt;&gt;"",Компоненты!R208,"")</f>
         <v/>
       </c>
       <c r="S199" t="str">
-        <f>IF(Компоненты!S199&lt;&gt;"",Компоненты!S199,"")</f>
+        <f>IF(Компоненты!S208&lt;&gt;"",Компоненты!S208,"")</f>
         <v/>
       </c>
       <c r="T199" t="str">
-        <f>IF(Компоненты!T199&lt;&gt;"",Компоненты!T199,"")</f>
+        <f>IF(Компоненты!T208&lt;&gt;"",Компоненты!T208,"")</f>
         <v/>
       </c>
       <c r="U199" t="str">
-        <f>IF(Компоненты!U199&lt;&gt;"",Компоненты!U199,"")</f>
+        <f>IF(Компоненты!U208&lt;&gt;"",Компоненты!U208,"")</f>
         <v/>
       </c>
     </row>
     <row r="200" spans="2:21">
       <c r="B200" t="str">
-        <f>IF(Компоненты!B200&lt;&gt;"",Компоненты!B200,"")</f>
+        <f>IF(Компоненты!B209&lt;&gt;"",Компоненты!B209,"")</f>
         <v/>
       </c>
       <c r="C200" t="str">
-        <f>IF(Компоненты!C200&lt;&gt;"",Компоненты!C200,"")</f>
+        <f>IF(Компоненты!C209&lt;&gt;"",Компоненты!C209,"")</f>
         <v/>
       </c>
       <c r="D200" t="str">
-        <f>IF(Компоненты!D200&lt;&gt;"",Компоненты!D200,"")</f>
+        <f>IF(Компоненты!D209&lt;&gt;"",Компоненты!D209,"")</f>
         <v/>
       </c>
       <c r="E200" t="str">
-        <f>IF(Компоненты!E200&lt;&gt;"",Компоненты!E200,"")</f>
+        <f>IF(Компоненты!E209&lt;&gt;"",Компоненты!E209,"")</f>
         <v/>
       </c>
       <c r="F200" t="str">
-        <f>IF(Компоненты!F200&lt;&gt;"",Компоненты!F200,"")</f>
+        <f>IF(Компоненты!F209&lt;&gt;"",Компоненты!F209,"")</f>
         <v/>
       </c>
       <c r="G200" t="str">
-        <f>IF(Компоненты!G200&lt;&gt;"",Компоненты!G200,"")</f>
+        <f>IF(Компоненты!G209&lt;&gt;"",Компоненты!G209,"")</f>
         <v/>
       </c>
       <c r="H200" t="str">
-        <f>IF(Компоненты!H200&lt;&gt;"",Компоненты!H200,"")</f>
+        <f>IF(Компоненты!H209&lt;&gt;"",Компоненты!H209,"")</f>
         <v/>
       </c>
       <c r="I200" t="str">
-        <f>IF(Компоненты!I200&lt;&gt;"",Компоненты!I200,"")</f>
+        <f>IF(Компоненты!I209&lt;&gt;"",Компоненты!I209,"")</f>
         <v/>
       </c>
       <c r="J200" t="str">
-        <f>IF(Компоненты!J200&lt;&gt;"",Компоненты!J200,"")</f>
+        <f>IF(Компоненты!J209&lt;&gt;"",Компоненты!J209,"")</f>
         <v/>
       </c>
       <c r="K200" t="str">
-        <f>IF(Компоненты!K200&lt;&gt;"",Компоненты!K200,"")</f>
+        <f>IF(Компоненты!K209&lt;&gt;"",Компоненты!K209,"")</f>
         <v/>
       </c>
       <c r="L200" t="str">
-        <f>IF(Компоненты!L200&lt;&gt;"",Компоненты!L200,"")</f>
+        <f>IF(Компоненты!L209&lt;&gt;"",Компоненты!L209,"")</f>
         <v/>
       </c>
       <c r="M200" t="str">
-        <f>IF(Компоненты!M200&lt;&gt;"",Компоненты!M200,"")</f>
+        <f>IF(Компоненты!M209&lt;&gt;"",Компоненты!M209,"")</f>
         <v/>
       </c>
       <c r="N200" t="str">
-        <f>IF(Компоненты!N200&lt;&gt;"",Компоненты!N200,"")</f>
+        <f>IF(Компоненты!N209&lt;&gt;"",Компоненты!N209,"")</f>
         <v/>
       </c>
       <c r="O200" t="str">
-        <f>IF(Компоненты!O200&lt;&gt;"",Компоненты!O200,"")</f>
+        <f>IF(Компоненты!O209&lt;&gt;"",Компоненты!O209,"")</f>
         <v/>
       </c>
       <c r="P200" t="str">
-        <f>IF(Компоненты!P200&lt;&gt;"",Компоненты!P200,"")</f>
+        <f>IF(Компоненты!P209&lt;&gt;"",Компоненты!P209,"")</f>
         <v/>
       </c>
       <c r="Q200" t="str">
-        <f>IF(Компоненты!Q200&lt;&gt;"",Компоненты!Q200,"")</f>
+        <f>IF(Компоненты!Q209&lt;&gt;"",Компоненты!Q209,"")</f>
         <v/>
       </c>
       <c r="R200" t="str">
-        <f>IF(Компоненты!R200&lt;&gt;"",Компоненты!R200,"")</f>
+        <f>IF(Компоненты!R209&lt;&gt;"",Компоненты!R209,"")</f>
         <v/>
       </c>
       <c r="S200" t="str">
-        <f>IF(Компоненты!S200&lt;&gt;"",Компоненты!S200,"")</f>
+        <f>IF(Компоненты!S209&lt;&gt;"",Компоненты!S209,"")</f>
         <v/>
       </c>
       <c r="T200" t="str">
-        <f>IF(Компоненты!T200&lt;&gt;"",Компоненты!T200,"")</f>
+        <f>IF(Компоненты!T209&lt;&gt;"",Компоненты!T209,"")</f>
         <v/>
       </c>
       <c r="U200" t="str">
-        <f>IF(Компоненты!U200&lt;&gt;"",Компоненты!U200,"")</f>
+        <f>IF(Компоненты!U209&lt;&gt;"",Компоненты!U209,"")</f>
         <v/>
       </c>
     </row>

</xml_diff>